<commit_message>
added fisheries catch to prep
</commit_message>
<xml_diff>
--- a/prep_whi/data_layers_WH.xlsx
+++ b/prep_whi/data_layers_WH.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="880" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="2960" yWindow="3480" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="data_layers_WH.csv" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="826" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="501">
   <si>
     <t>Goal</t>
   </si>
@@ -1960,8 +1960,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A32" workbookViewId="0">
-      <selection activeCell="L50" sqref="L50"/>
+    <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
+      <selection activeCell="F110" sqref="F110"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4960,9 +4960,7 @@
       <c r="A91" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="B91" s="4" t="s">
-        <v>62</v>
-      </c>
+      <c r="B91" s="4"/>
       <c r="C91" s="14" t="s">
         <v>397</v>
       </c>
@@ -4993,9 +4991,7 @@
       <c r="A92" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="B92" s="4" t="s">
-        <v>62</v>
-      </c>
+      <c r="B92" s="4"/>
       <c r="C92" s="14" t="s">
         <v>402</v>
       </c>
@@ -5028,9 +5024,7 @@
       <c r="A93" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="B93" s="4" t="s">
-        <v>62</v>
-      </c>
+      <c r="B93" s="4"/>
       <c r="C93" s="14" t="s">
         <v>407</v>
       </c>
@@ -5061,9 +5055,7 @@
       <c r="A94" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="B94" s="4" t="s">
-        <v>62</v>
-      </c>
+      <c r="B94" s="4"/>
       <c r="C94" s="14" t="s">
         <v>28</v>
       </c>

</xml_diff>

<commit_message>
added data to prep tourism
</commit_message>
<xml_diff>
--- a/prep_whi/data_layers_WH.xlsx
+++ b/prep_whi/data_layers_WH.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2960" yWindow="3480" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="data_layers_WH.csv" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="822" uniqueCount="501">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="825" uniqueCount="502">
   <si>
     <t>Goal</t>
   </si>
@@ -1478,9 +1478,6 @@
     <t>(not sure if this is being included in model - will need to ask working group)</t>
   </si>
   <si>
-    <t>Trying to get just West Hawaii estimates</t>
-  </si>
-  <si>
     <t xml:space="preserve">Lisa Meric - up to date layer - Douglas Harger also mapping out </t>
   </si>
   <si>
@@ -1530,6 +1527,12 @@
   </si>
   <si>
     <t>Coral bleaching</t>
+  </si>
+  <si>
+    <t>http://www.hawaiitourismauthority.org/research/reports/annual-visitor-research/</t>
+  </si>
+  <si>
+    <t>Kona side visitor days, Hawaii Island visitor revenue, and average daily spending.</t>
   </si>
 </sst>
 </file>
@@ -1961,7 +1964,7 @@
   <dimension ref="A1:Z105"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A90" workbookViewId="0">
-      <selection activeCell="F110" sqref="F110"/>
+      <selection activeCell="L106" sqref="L106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2296,7 +2299,7 @@
         <v>479</v>
       </c>
       <c r="N9" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
@@ -2326,7 +2329,7 @@
         <v>465</v>
       </c>
       <c r="N10" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
@@ -2354,10 +2357,10 @@
         <v>466</v>
       </c>
       <c r="N11" t="s">
+        <v>485</v>
+      </c>
+      <c r="O11" t="s">
         <v>486</v>
-      </c>
-      <c r="O11" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="48" hidden="1" x14ac:dyDescent="0.2">
@@ -2469,7 +2472,7 @@
         <v>79</v>
       </c>
       <c r="N14" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="64" x14ac:dyDescent="0.2">
@@ -2907,7 +2910,7 @@
         <v>480</v>
       </c>
       <c r="N27" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
     </row>
     <row r="28" spans="1:19" x14ac:dyDescent="0.2">
@@ -3054,7 +3057,7 @@
         <v>161</v>
       </c>
       <c r="N31" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
     </row>
     <row r="32" spans="1:19" x14ac:dyDescent="0.2">
@@ -3285,10 +3288,10 @@
         <v>468</v>
       </c>
       <c r="N37" s="16" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="O37" s="16" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="P37" s="16"/>
       <c r="Q37" s="16"/>
@@ -3318,7 +3321,7 @@
       </c>
       <c r="M38" s="17"/>
       <c r="N38" s="16" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="O38" s="16"/>
       <c r="P38" s="16"/>
@@ -3604,10 +3607,10 @@
         <v>465</v>
       </c>
       <c r="N46" t="s">
+        <v>493</v>
+      </c>
+      <c r="O46" t="s">
         <v>494</v>
-      </c>
-      <c r="O46" t="s">
-        <v>495</v>
       </c>
       <c r="Y46">
         <v>4</v>
@@ -3640,19 +3643,19 @@
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
       <c r="K47" s="5" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="L47" s="18" t="s">
         <v>21</v>
       </c>
       <c r="M47" s="8" t="s">
+        <v>497</v>
+      </c>
+      <c r="N47" t="s">
         <v>498</v>
       </c>
-      <c r="N47" t="s">
-        <v>499</v>
-      </c>
       <c r="O47" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="Y47">
         <v>4</v>
@@ -3739,7 +3742,7 @@
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="5" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="D50" s="4"/>
       <c r="E50" s="4"/>
@@ -5400,7 +5403,7 @@
       <c r="L103" s="7"/>
       <c r="M103" s="7"/>
     </row>
-    <row r="104" spans="1:26" ht="32" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:26" ht="48" x14ac:dyDescent="0.2">
       <c r="A104" s="4" t="s">
         <v>445</v>
       </c>
@@ -5431,9 +5434,14 @@
         <v>459</v>
       </c>
       <c r="L104" s="7"/>
-      <c r="M104" s="7"/>
-    </row>
-    <row r="105" spans="1:26" ht="32" x14ac:dyDescent="0.2">
+      <c r="M104" s="8" t="s">
+        <v>501</v>
+      </c>
+      <c r="N104" t="s">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="105" spans="1:26" ht="48" x14ac:dyDescent="0.2">
       <c r="A105" s="4" t="s">
         <v>445</v>
       </c>
@@ -5465,7 +5473,10 @@
         <v>21</v>
       </c>
       <c r="M105" s="8" t="s">
-        <v>483</v>
+        <v>501</v>
+      </c>
+      <c r="N105" t="s">
+        <v>500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated cp habitat extent
</commit_message>
<xml_diff>
--- a/prep_whi/data_layers_WH.xlsx
+++ b/prep_whi/data_layers_WH.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data_layers_WH.csv" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="831" uniqueCount="508">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="557">
   <si>
     <t>Goal</t>
   </si>
@@ -159,9 +159,6 @@
     <t>HAB</t>
   </si>
   <si>
-    <t>wetlands</t>
-  </si>
-  <si>
     <t>wetlands_OHI</t>
   </si>
   <si>
@@ -636,9 +633,6 @@
     <t>DBEDT average resident population per county</t>
   </si>
   <si>
-    <t xml:space="preserve">Is there data available on intertidal habitats for West Hawaii? </t>
-  </si>
-  <si>
     <t>forest/watershed health</t>
   </si>
   <si>
@@ -654,9 +648,6 @@
     <t>TNC 2010</t>
   </si>
   <si>
-    <t>Is there an updated data set? This data is at the Island scale, we need to get to the West Hawaii scale. Maybe use NOAA CCAP data.</t>
-  </si>
-  <si>
     <t>ocean acidification</t>
   </si>
   <si>
@@ -1552,13 +1543,169 @@
   </si>
   <si>
     <t>updating website, adding content and communication</t>
+  </si>
+  <si>
+    <t xml:space="preserve">coastal development layers but fishpond walls are not differentiated from development, armored shorelines - OTP layer - cummulative impacts also, ESI and NOAA habitat maps </t>
+  </si>
+  <si>
+    <t>Molokai fishponds needs to be removed</t>
+  </si>
+  <si>
+    <t>Reference: % of shoreline armored for intertidal pressure</t>
+  </si>
+  <si>
+    <t>Joey working on updating</t>
+  </si>
+  <si>
+    <t>landfire.gov</t>
+  </si>
+  <si>
+    <t>also look at HCA for maps of native vs non-native</t>
+  </si>
+  <si>
+    <t>development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">National Fish Habiat Action Plan - Dept of Interior - freshwater focused - Joey has layers </t>
+  </si>
+  <si>
+    <t>percent of watersheds that are developed (only for WH). 1992 is oldest time step</t>
+  </si>
+  <si>
+    <t>will current development to refrence time series development</t>
+  </si>
+  <si>
+    <t>USGS vegatation cover types, one time step but modeled several time steps for plant growth, 2001 was latest assessment but coming out with 2015 base map</t>
+  </si>
+  <si>
+    <t>Joey is working on updating</t>
+  </si>
+  <si>
+    <t>Joey has a map with aquaculture and names of companies</t>
+  </si>
+  <si>
+    <t xml:space="preserve">how to reference this pressure? % of coastline that is exposed to aquaculture apperations </t>
+  </si>
+  <si>
+    <t>aquaculture projections and permits - joey has this file - future proposed aquaculture facilities, Office of Conservation and Coastal Lands</t>
+  </si>
+  <si>
+    <t>use sum of catch per area (Joey has through 2015 yearly), 2013 they reported at finer scale for Hawaii Island - Joey has reported block maps</t>
+  </si>
+  <si>
+    <t>Joey will send me data</t>
+  </si>
+  <si>
+    <t xml:space="preserve">percent of area in high , med, low fishing intensity for shore and boat , joey has commercial catch layers we can use too - Joey can send to me too, </t>
+  </si>
+  <si>
+    <t>Joey wil send me areas of fishing intensity</t>
+  </si>
+  <si>
+    <t>this is intertidal layer</t>
+  </si>
+  <si>
+    <t>joey will combine this into one pressure layer and give % of area in high impact and low impact from dredging and benthic structures</t>
+  </si>
+  <si>
+    <t xml:space="preserve">could summarize by habitat type - </t>
+  </si>
+  <si>
+    <t>joey will update - *joey will update to each habitat % of area impacted of reefs and softbottom</t>
+  </si>
+  <si>
+    <t>presence data for invasives (not presence/absence)</t>
+  </si>
+  <si>
+    <t>fish and algae are separate layers; mangroves are separated as a layer</t>
+  </si>
+  <si>
+    <t>Eva - will follow up with brian; eva will update invasive laysers, mangroves/coastline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Jonatha has spatial model of predicted roi abundance - data exists to model invasive species - </t>
+  </si>
+  <si>
+    <t xml:space="preserve">how to stadardize: total load and standardize by length of coastline </t>
+  </si>
+  <si>
+    <t>Joey is updating</t>
+  </si>
+  <si>
+    <t>may use watershed land use here</t>
+  </si>
+  <si>
+    <t>may use watershed land use here (area of golf course by region); how to standardize - distance to shoreline or watershed area</t>
+  </si>
+  <si>
+    <t>based on map that DAR generated - # of debris pieces and weighted by size class (ask brian for reference for this data); reference - total by region divided by coastline/ use Niihoa as reference - not getting cleaned</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eva will update (ask brian for point data) </t>
+  </si>
+  <si>
+    <t>aerial surveys from 2006 and 2009 for marine debris for big debris from helicoper - lower spatial scale</t>
+  </si>
+  <si>
+    <t>OTP layer is commerical shipping only</t>
+  </si>
+  <si>
+    <t>Joey has small boat harbors so could assess risk for small boat groundings also</t>
+  </si>
+  <si>
+    <t>database of grounding location - EVA ask DAR and follow up with Joey</t>
+  </si>
+  <si>
+    <t>Boat traffic data from dobor</t>
+  </si>
+  <si>
+    <t>total area in high, medium, low risk of groundings for hardbottom habitat</t>
+  </si>
+  <si>
+    <t>ship based pollution by habitat type - soft and reef</t>
+  </si>
+  <si>
+    <t>How to reference: total impact summed by region/length of coastline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eva wil look at tourism data for this and human use </t>
+  </si>
+  <si>
+    <t>think about West Hawaii dolphin tours, etc...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESI has tourism/ soeco layer </t>
+  </si>
+  <si>
+    <t>standardizing pressures and updating pressure layers with Joey Lecky at NOAA</t>
+  </si>
+  <si>
+    <t>12/18/2017</t>
+  </si>
+  <si>
+    <t>habitats</t>
+  </si>
+  <si>
+    <t>12/22/2017</t>
+  </si>
+  <si>
+    <t>extracted ESI beach data, extracted NOAA 2010 wetland data for within 1km of coastline (trend from ccap may be a bit off, the resolution from 2005 is poor so the changes may reflex differences in resolution, looking to the wetland study for trend and condition</t>
+  </si>
+  <si>
+    <t>coastal wetland extent</t>
+  </si>
+  <si>
+    <t>12/26/2017</t>
+  </si>
+  <si>
+    <t xml:space="preserve">updated cp_extent layer updated, need to updated mhi reef exent layer </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -1583,6 +1730,14 @@
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="5">
@@ -1650,7 +1805,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1709,9 +1864,6 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -1732,6 +1884,12 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="17" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -2010,24 +2168,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA103"/>
+  <dimension ref="A1:AA104"/>
   <sheetViews>
-    <sheetView topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.83203125" style="20" customWidth="1"/>
-    <col min="2" max="2" width="7.83203125" style="20" customWidth="1"/>
+    <col min="2" max="2" width="2.5" style="20" customWidth="1"/>
     <col min="3" max="3" width="17.83203125" style="21" customWidth="1"/>
-    <col min="4" max="4" width="31.83203125" style="20" customWidth="1"/>
-    <col min="5" max="5" width="27.5" style="20" customWidth="1"/>
+    <col min="4" max="4" width="22.5" style="20" customWidth="1"/>
+    <col min="5" max="5" width="20.1640625" style="20" customWidth="1"/>
     <col min="6" max="6" width="48" style="21" customWidth="1"/>
     <col min="7" max="7" width="16.33203125" style="20" customWidth="1"/>
-    <col min="8" max="8" width="10" style="20" customWidth="1"/>
-    <col min="9" max="9" width="10.5" style="20" customWidth="1"/>
-    <col min="10" max="10" width="11.1640625" style="20" customWidth="1"/>
+    <col min="8" max="8" width="6.1640625" style="20" customWidth="1"/>
+    <col min="9" max="9" width="6.6640625" style="20" customWidth="1"/>
+    <col min="10" max="10" width="6.83203125" style="20" customWidth="1"/>
     <col min="11" max="11" width="37.5" style="21" customWidth="1"/>
     <col min="12" max="12" width="30.33203125" customWidth="1"/>
     <col min="13" max="14" width="25.5" customWidth="1"/>
@@ -2068,17 +2226,17 @@
         <v>10</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>445</v>
+        <v>442</v>
       </c>
       <c r="M1" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="28"/>
-      <c r="O1" s="27" t="s">
-        <v>483</v>
-      </c>
-      <c r="P1" s="27" t="s">
-        <v>484</v>
+      <c r="N1" s="27"/>
+      <c r="O1" s="26" t="s">
+        <v>480</v>
+      </c>
+      <c r="P1" s="26" t="s">
+        <v>481</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="48" x14ac:dyDescent="0.2">
@@ -2115,9 +2273,9 @@
         <v>21</v>
       </c>
       <c r="M2" s="7" t="s">
-        <v>447</v>
-      </c>
-      <c r="N2" s="29"/>
+        <v>444</v>
+      </c>
+      <c r="N2" s="28"/>
     </row>
     <row r="3" spans="1:16" ht="48" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -2153,7 +2311,7 @@
       </c>
       <c r="L3" s="7"/>
       <c r="M3" s="7"/>
-      <c r="N3" s="29"/>
+      <c r="N3" s="28"/>
     </row>
     <row r="4" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -2189,7 +2347,7 @@
       </c>
       <c r="L4" s="7"/>
       <c r="M4" s="7"/>
-      <c r="N4" s="29"/>
+      <c r="N4" s="28"/>
     </row>
     <row r="5" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -2227,7 +2385,7 @@
       <c r="M5" s="10" t="s">
         <v>40</v>
       </c>
-      <c r="N5" s="30"/>
+      <c r="N5" s="29"/>
     </row>
     <row r="6" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -2237,16 +2395,16 @@
         <v>42</v>
       </c>
       <c r="C6" s="5" t="s">
+        <v>554</v>
+      </c>
+      <c r="D6" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="E6" s="4" t="s">
+      <c r="F6" s="5" t="s">
         <v>45</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>46</v>
       </c>
       <c r="G6" s="4" t="s">
         <v>17</v>
@@ -2259,11 +2417,11 @@
       </c>
       <c r="J6" s="4"/>
       <c r="K6" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L6" s="7"/>
       <c r="M6" s="7"/>
-      <c r="N6" s="29"/>
+      <c r="N6" s="28"/>
     </row>
     <row r="7" spans="1:16" ht="69" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -2273,16 +2431,16 @@
         <v>42</v>
       </c>
       <c r="C7" s="5" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="D7" s="4" t="s">
+      <c r="E7" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="E7" s="4" t="s">
+      <c r="F7" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="G7" s="4" t="s">
         <v>17</v>
@@ -2295,11 +2453,11 @@
       </c>
       <c r="J7" s="4"/>
       <c r="K7" s="5" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="L7" s="7"/>
       <c r="M7" s="7"/>
-      <c r="N7" s="29"/>
+      <c r="N7" s="28"/>
     </row>
     <row r="8" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
@@ -2309,16 +2467,16 @@
         <v>42</v>
       </c>
       <c r="C8" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="D8" s="4" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="E8" s="4" t="s">
+      <c r="F8" s="5" t="s">
         <v>55</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>56</v>
       </c>
       <c r="G8" s="4" t="s">
         <v>17</v>
@@ -2327,15 +2485,15 @@
       <c r="I8" s="4"/>
       <c r="J8" s="4"/>
       <c r="K8" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="L8" s="7" t="s">
         <v>21</v>
       </c>
       <c r="M8" s="8" t="s">
-        <v>58</v>
-      </c>
-      <c r="N8" s="31"/>
+        <v>57</v>
+      </c>
+      <c r="N8" s="30"/>
     </row>
     <row r="9" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
@@ -2345,7 +2503,7 @@
         <v>42</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D9" s="4"/>
       <c r="E9" s="4"/>
@@ -2359,11 +2517,11 @@
         <v>21</v>
       </c>
       <c r="M9" s="8" t="s">
-        <v>499</v>
-      </c>
-      <c r="N9" s="31"/>
+        <v>496</v>
+      </c>
+      <c r="N9" s="30"/>
       <c r="O9" t="s">
-        <v>463</v>
+        <v>460</v>
       </c>
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.2">
@@ -2374,12 +2532,12 @@
         <v>42</v>
       </c>
       <c r="C10" s="5" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D10" s="4"/>
       <c r="E10" s="4"/>
       <c r="F10" s="5" t="s">
-        <v>448</v>
+        <v>445</v>
       </c>
       <c r="G10" s="4"/>
       <c r="H10" s="4"/>
@@ -2390,11 +2548,11 @@
         <v>21</v>
       </c>
       <c r="M10" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="N10" s="29"/>
+        <v>443</v>
+      </c>
+      <c r="N10" s="28"/>
       <c r="O10" t="s">
-        <v>464</v>
+        <v>461</v>
       </c>
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.2">
@@ -2405,7 +2563,7 @@
         <v>42</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D11" s="4"/>
       <c r="E11" s="4"/>
@@ -2419,32 +2577,32 @@
         <v>21</v>
       </c>
       <c r="M11" s="7" t="s">
-        <v>447</v>
-      </c>
-      <c r="N11" s="29"/>
+        <v>444</v>
+      </c>
+      <c r="N11" s="28"/>
       <c r="O11" t="s">
-        <v>465</v>
+        <v>462</v>
       </c>
       <c r="P11" t="s">
-        <v>466</v>
+        <v>463</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="48" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="5" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="E12" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="5" t="s">
         <v>64</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F12" s="5" t="s">
-        <v>65</v>
       </c>
       <c r="G12" s="4" t="s">
         <v>17</v>
@@ -2457,30 +2615,30 @@
       </c>
       <c r="J12" s="4"/>
       <c r="K12" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="L12" s="7"/>
       <c r="M12" s="7"/>
-      <c r="N12" s="29"/>
+      <c r="N12" s="28"/>
     </row>
     <row r="13" spans="1:16" ht="32" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B13" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="C13" s="5" t="s">
         <v>66</v>
       </c>
-      <c r="C13" s="5" t="s">
+      <c r="D13" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="D13" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="E13" s="4" t="s">
+      <c r="F13" s="5" t="s">
         <v>69</v>
-      </c>
-      <c r="F13" s="5" t="s">
-        <v>70</v>
       </c>
       <c r="G13" s="4" t="s">
         <v>17</v>
@@ -2495,73 +2653,73 @@
         <v>38</v>
       </c>
       <c r="K13" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="L13" s="6"/>
       <c r="M13" s="7"/>
-      <c r="N13" s="29"/>
+      <c r="N13" s="28"/>
     </row>
     <row r="14" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
         <v>41</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>71</v>
+      </c>
+      <c r="D14" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="D14" s="4" t="s">
+      <c r="E14" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="E14" s="4" t="s">
+      <c r="F14" s="5" t="s">
         <v>74</v>
-      </c>
-      <c r="F14" s="5" t="s">
-        <v>75</v>
       </c>
       <c r="G14" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4" t="s">
+        <v>75</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="J14" s="4" t="s">
+      <c r="K14" s="5" t="s">
         <v>77</v>
-      </c>
-      <c r="K14" s="5" t="s">
-        <v>78</v>
       </c>
       <c r="L14" s="7" t="s">
         <v>21</v>
       </c>
       <c r="M14" s="8" t="s">
-        <v>79</v>
-      </c>
-      <c r="N14" s="31"/>
+        <v>78</v>
+      </c>
+      <c r="N14" s="30"/>
       <c r="O14" t="s">
-        <v>467</v>
+        <v>464</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>42</v>
       </c>
       <c r="C15" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="D15" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="E15" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="5" t="s">
         <v>82</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="F15" s="5" t="s">
-        <v>83</v>
       </c>
       <c r="G15" s="4"/>
       <c r="H15" s="4">
@@ -2572,132 +2730,132 @@
       </c>
       <c r="J15" s="4"/>
       <c r="K15" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="L15" s="7"/>
       <c r="M15" s="7"/>
-      <c r="N15" s="29"/>
+      <c r="N15" s="28"/>
     </row>
     <row r="16" spans="1:16" ht="64" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="D16" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="4" t="s">
+      <c r="E16" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="E16" s="4" t="s">
+      <c r="F16" s="5" t="s">
         <v>87</v>
-      </c>
-      <c r="F16" s="5" t="s">
-        <v>88</v>
       </c>
       <c r="G16" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J16" s="4"/>
       <c r="K16" s="5" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L16" s="6"/>
       <c r="M16" s="7"/>
-      <c r="N16" s="29"/>
+      <c r="N16" s="28"/>
     </row>
     <row r="17" spans="1:20" s="12" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A17" s="6" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B17" s="6"/>
       <c r="C17" s="10" t="s">
+        <v>89</v>
+      </c>
+      <c r="D17" s="6" t="s">
         <v>90</v>
       </c>
-      <c r="D17" s="6" t="s">
+      <c r="E17" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="E17" s="6" t="s">
+      <c r="F17" s="10" t="s">
         <v>92</v>
-      </c>
-      <c r="F17" s="10" t="s">
-        <v>93</v>
       </c>
       <c r="G17" s="6" t="s">
         <v>17</v>
       </c>
       <c r="H17" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J17" s="6"/>
       <c r="K17" s="10" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L17" s="6"/>
       <c r="M17" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="N17" s="32"/>
+        <v>94</v>
+      </c>
+      <c r="N17" s="31"/>
     </row>
     <row r="18" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" s="4"/>
       <c r="C18" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="D18" s="4" t="s">
+      <c r="E18" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="E18" s="4" t="s">
+      <c r="F18" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="F18" s="5" t="s">
+      <c r="G18" s="4" t="s">
         <v>99</v>
       </c>
-      <c r="G18" s="4" t="s">
-        <v>100</v>
-      </c>
       <c r="H18" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I18" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="J18" s="4"/>
       <c r="K18" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="L18" s="6"/>
       <c r="M18" s="7"/>
-      <c r="N18" s="29"/>
+      <c r="N18" s="28"/>
     </row>
     <row r="19" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="4"/>
       <c r="C19" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D19" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="D19" s="4" t="s">
+      <c r="E19" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="E19" s="4" t="s">
+      <c r="F19" s="5" t="s">
         <v>103</v>
-      </c>
-      <c r="F19" s="5" t="s">
-        <v>104</v>
       </c>
       <c r="G19" s="4" t="s">
         <v>17</v>
@@ -2706,28 +2864,28 @@
       <c r="I19" s="4"/>
       <c r="J19" s="4"/>
       <c r="K19" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L19" s="6"/>
       <c r="M19" s="7"/>
-      <c r="N19" s="29"/>
+      <c r="N19" s="28"/>
     </row>
     <row r="20" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A20" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B20" s="4"/>
       <c r="C20" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="F20" s="5" t="s">
         <v>107</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="F20" s="5" t="s">
-        <v>108</v>
       </c>
       <c r="G20" s="4" t="s">
         <v>17</v>
@@ -2739,31 +2897,31 @@
         <v>2011</v>
       </c>
       <c r="J20" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="K20" s="5" t="s">
         <v>109</v>
-      </c>
-      <c r="K20" s="5" t="s">
-        <v>110</v>
       </c>
       <c r="L20" s="6"/>
       <c r="M20" s="7"/>
-      <c r="N20" s="29"/>
+      <c r="N20" s="28"/>
     </row>
     <row r="21" spans="1:20" ht="32" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B21" s="4"/>
       <c r="C21" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D21" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F21" s="5" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="G21" s="4" t="s">
         <v>17</v>
@@ -2774,28 +2932,28 @@
       </c>
       <c r="J21" s="4"/>
       <c r="K21" s="5" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="L21" s="7"/>
       <c r="M21" s="7"/>
-      <c r="N21" s="29"/>
+      <c r="N21" s="28"/>
     </row>
     <row r="22" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A22" s="4" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D22" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
         <v>114</v>
       </c>
-      <c r="E22" s="4" t="s">
+      <c r="F22" s="5" t="s">
         <v>115</v>
-      </c>
-      <c r="F22" s="5" t="s">
-        <v>116</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>17</v>
@@ -2804,30 +2962,30 @@
       <c r="I22" s="4"/>
       <c r="J22" s="4"/>
       <c r="K22" s="5" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="L22" s="7"/>
       <c r="M22" s="7"/>
-      <c r="N22" s="29"/>
+      <c r="N22" s="28"/>
     </row>
     <row r="23" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A23" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="C23" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C23" s="5" t="s">
+      <c r="D23" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="D23" s="4" t="s">
+      <c r="E23" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="E23" s="4" t="s">
+      <c r="F23" s="5" t="s">
         <v>121</v>
-      </c>
-      <c r="F23" s="5" t="s">
-        <v>122</v>
       </c>
       <c r="G23" s="4" t="s">
         <v>17</v>
@@ -2840,30 +2998,30 @@
       </c>
       <c r="J23" s="4"/>
       <c r="K23" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L23" s="7"/>
       <c r="M23" s="7"/>
-      <c r="N23" s="29"/>
+      <c r="N23" s="28"/>
     </row>
     <row r="24" spans="1:20" ht="64" x14ac:dyDescent="0.2">
       <c r="A24" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B24" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B24" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="C24" s="5" t="s">
+        <v>123</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="D24" s="4" t="s">
+      <c r="E24" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="E24" s="4" t="s">
+      <c r="F24" s="5" t="s">
         <v>126</v>
-      </c>
-      <c r="F24" s="5" t="s">
-        <v>127</v>
       </c>
       <c r="G24" s="4" t="s">
         <v>17</v>
@@ -2876,30 +3034,30 @@
       </c>
       <c r="J24" s="4"/>
       <c r="K24" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="L24" s="7"/>
       <c r="M24" s="7"/>
-      <c r="N24" s="29"/>
+      <c r="N24" s="28"/>
     </row>
     <row r="25" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A25" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B25" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B25" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="C25" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="D25" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="D25" s="4" t="s">
+      <c r="E25" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E25" s="4" t="s">
+      <c r="F25" s="5" t="s">
         <v>131</v>
-      </c>
-      <c r="F25" s="5" t="s">
-        <v>132</v>
       </c>
       <c r="G25" s="4" t="s">
         <v>17</v>
@@ -2910,30 +3068,30 @@
       </c>
       <c r="J25" s="4"/>
       <c r="K25" s="5" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="L25" s="7"/>
       <c r="M25" s="7"/>
-      <c r="N25" s="29"/>
+      <c r="N25" s="28"/>
     </row>
     <row r="26" spans="1:20" ht="80" x14ac:dyDescent="0.2">
       <c r="A26" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B26" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="C26" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C26" s="5" t="s">
+      <c r="D26" s="4" t="s">
         <v>135</v>
       </c>
-      <c r="D26" s="4" t="s">
+      <c r="E26" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="F26" s="5" t="s">
         <v>136</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="F26" s="5" t="s">
-        <v>137</v>
       </c>
       <c r="G26" s="4" t="s">
         <v>17</v>
@@ -2946,30 +3104,30 @@
       </c>
       <c r="J26" s="4"/>
       <c r="K26" s="5" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="L26" s="7"/>
       <c r="M26" s="7"/>
-      <c r="N26" s="29"/>
+      <c r="N26" s="28"/>
     </row>
     <row r="27" spans="1:20" ht="96" x14ac:dyDescent="0.2">
       <c r="A27" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C27" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="D27" s="4" t="s">
         <v>139</v>
       </c>
-      <c r="D27" s="4" t="s">
+      <c r="E27" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="F27" s="5" t="s">
         <v>140</v>
-      </c>
-      <c r="E27" s="4" t="s">
-        <v>140</v>
-      </c>
-      <c r="F27" s="5" t="s">
-        <v>141</v>
       </c>
       <c r="G27" s="4" t="s">
         <v>17</v>
@@ -2982,37 +3140,37 @@
       </c>
       <c r="J27" s="4"/>
       <c r="K27" s="5" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="L27" s="7" t="s">
         <v>21</v>
       </c>
       <c r="M27" s="8" t="s">
-        <v>460</v>
-      </c>
-      <c r="N27" s="31"/>
+        <v>457</v>
+      </c>
+      <c r="N27" s="30"/>
       <c r="O27" t="s">
-        <v>468</v>
+        <v>465</v>
       </c>
     </row>
     <row r="28" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A28" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C28" s="5" t="s">
+        <v>142</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="D28" s="4" t="s">
+      <c r="E28" s="4" t="s">
+        <v>143</v>
+      </c>
+      <c r="F28" s="5" t="s">
         <v>144</v>
-      </c>
-      <c r="E28" s="4" t="s">
-        <v>144</v>
-      </c>
-      <c r="F28" s="5" t="s">
-        <v>145</v>
       </c>
       <c r="G28" s="4" t="s">
         <v>17</v>
@@ -3025,30 +3183,30 @@
       </c>
       <c r="J28" s="4"/>
       <c r="K28" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L28" s="7"/>
       <c r="M28" s="7"/>
-      <c r="N28" s="29"/>
+      <c r="N28" s="28"/>
     </row>
     <row r="29" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C29" s="5" t="s">
+        <v>146</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>147</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="E29" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="F29" s="5" t="s">
         <v>148</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>148</v>
-      </c>
-      <c r="F29" s="5" t="s">
-        <v>149</v>
       </c>
       <c r="G29" s="4" t="s">
         <v>17</v>
@@ -3061,30 +3219,30 @@
       </c>
       <c r="J29" s="4"/>
       <c r="K29" s="5" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="L29" s="7"/>
       <c r="M29" s="7"/>
-      <c r="N29" s="29"/>
+      <c r="N29" s="28"/>
     </row>
     <row r="30" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A30" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B30" s="4" t="s">
         <v>150</v>
       </c>
-      <c r="B30" s="4" t="s">
+      <c r="C30" s="5" t="s">
         <v>151</v>
       </c>
-      <c r="C30" s="5" t="s">
+      <c r="D30" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="D30" s="4" t="s">
+      <c r="E30" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="E30" s="4" t="s">
-        <v>154</v>
-      </c>
       <c r="F30" s="5" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="G30" s="4" t="s">
         <v>17</v>
@@ -3097,30 +3255,30 @@
       </c>
       <c r="J30" s="4"/>
       <c r="K30" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L30" s="7"/>
       <c r="M30" s="7"/>
-      <c r="N30" s="29"/>
+      <c r="N30" s="28"/>
     </row>
     <row r="31" spans="1:20" ht="32" x14ac:dyDescent="0.2">
       <c r="A31" s="4" t="s">
+        <v>149</v>
+      </c>
+      <c r="B31" s="13" t="s">
         <v>150</v>
       </c>
-      <c r="B31" s="13" t="s">
-        <v>151</v>
-      </c>
       <c r="C31" s="14" t="s">
+        <v>155</v>
+      </c>
+      <c r="D31" s="13" t="s">
         <v>156</v>
       </c>
-      <c r="D31" s="13" t="s">
+      <c r="E31" s="13" t="s">
         <v>157</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="F31" s="14" t="s">
         <v>158</v>
-      </c>
-      <c r="F31" s="14" t="s">
-        <v>159</v>
       </c>
       <c r="G31" s="13" t="s">
         <v>17</v>
@@ -3133,37 +3291,37 @@
       </c>
       <c r="J31" s="13"/>
       <c r="K31" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L31" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M31" s="26" t="s">
-        <v>161</v>
-      </c>
-      <c r="N31" s="33"/>
+      <c r="M31" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="N31" s="32"/>
       <c r="O31" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
     </row>
     <row r="32" spans="1:20" x14ac:dyDescent="0.2">
       <c r="A32" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C32" s="5" t="s">
         <v>28</v>
       </c>
       <c r="D32" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="E32" s="4" t="s">
         <v>163</v>
       </c>
-      <c r="E32" s="4" t="s">
+      <c r="F32" s="5" t="s">
         <v>164</v>
-      </c>
-      <c r="F32" s="5" t="s">
-        <v>165</v>
       </c>
       <c r="G32" s="4" t="s">
         <v>17</v>
@@ -3176,13 +3334,13 @@
       </c>
       <c r="J32" s="4"/>
       <c r="K32" s="5" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L32" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="M32" s="26"/>
-      <c r="N32" s="33"/>
+      <c r="M32" s="37"/>
+      <c r="N32" s="32"/>
       <c r="O32" s="16"/>
       <c r="P32" s="16"/>
       <c r="Q32" s="16"/>
@@ -3192,22 +3350,22 @@
     </row>
     <row r="33" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A33" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B33" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C33" s="14" t="s">
+        <v>165</v>
+      </c>
+      <c r="D33" s="13" t="s">
         <v>166</v>
       </c>
-      <c r="D33" s="13" t="s">
+      <c r="E33" s="13" t="s">
         <v>167</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="F33" s="14" t="s">
         <v>168</v>
-      </c>
-      <c r="F33" s="14" t="s">
-        <v>169</v>
       </c>
       <c r="G33" s="13" t="s">
         <v>17</v>
@@ -3220,13 +3378,13 @@
       </c>
       <c r="J33" s="13"/>
       <c r="K33" s="14" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="L33" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="M33" s="26"/>
-      <c r="N33" s="33"/>
+      <c r="M33" s="37"/>
+      <c r="N33" s="32"/>
       <c r="O33" s="16"/>
       <c r="P33" s="16"/>
       <c r="Q33" s="16"/>
@@ -3236,22 +3394,22 @@
     </row>
     <row r="34" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A34" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B34" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C34" s="14" t="s">
+        <v>169</v>
+      </c>
+      <c r="D34" s="13" t="s">
         <v>170</v>
       </c>
-      <c r="D34" s="13" t="s">
+      <c r="E34" s="13" t="s">
         <v>171</v>
       </c>
-      <c r="E34" s="13" t="s">
+      <c r="F34" s="14" t="s">
         <v>172</v>
-      </c>
-      <c r="F34" s="14" t="s">
-        <v>173</v>
       </c>
       <c r="G34" s="13" t="s">
         <v>17</v>
@@ -3264,13 +3422,13 @@
       </c>
       <c r="J34" s="13"/>
       <c r="K34" s="14" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="L34" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="M34" s="26"/>
-      <c r="N34" s="33"/>
+      <c r="M34" s="37"/>
+      <c r="N34" s="32"/>
       <c r="O34" s="16"/>
       <c r="P34" s="16"/>
       <c r="Q34" s="16"/>
@@ -3280,22 +3438,22 @@
     </row>
     <row r="35" spans="1:27" ht="32" x14ac:dyDescent="0.2">
       <c r="A35" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B35" s="13" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C35" s="14" t="s">
+        <v>174</v>
+      </c>
+      <c r="D35" s="13" t="s">
         <v>175</v>
       </c>
-      <c r="D35" s="13" t="s">
+      <c r="E35" s="13" t="s">
         <v>176</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="F35" s="14" t="s">
         <v>177</v>
-      </c>
-      <c r="F35" s="14" t="s">
-        <v>178</v>
       </c>
       <c r="G35" s="13" t="s">
         <v>17</v>
@@ -3308,13 +3466,13 @@
       </c>
       <c r="J35" s="13"/>
       <c r="K35" s="14" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="L35" s="15" t="s">
         <v>21</v>
       </c>
-      <c r="M35" s="26"/>
-      <c r="N35" s="33"/>
+      <c r="M35" s="37"/>
+      <c r="N35" s="32"/>
       <c r="O35" s="16"/>
       <c r="P35" s="16"/>
       <c r="Q35" s="16"/>
@@ -3324,29 +3482,29 @@
     </row>
     <row r="36" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A36" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B36" s="13"/>
       <c r="C36" s="14" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="D36" s="13"/>
       <c r="E36" s="13"/>
       <c r="F36" s="14" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G36" s="13"/>
       <c r="H36" s="13"/>
       <c r="I36" s="13"/>
       <c r="J36" s="13"/>
       <c r="K36" s="14" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="L36" s="15" t="s">
         <v>21</v>
       </c>
       <c r="M36" s="17"/>
-      <c r="N36" s="33"/>
+      <c r="N36" s="32"/>
       <c r="O36" s="16"/>
       <c r="P36" s="16"/>
       <c r="Q36" s="16"/>
@@ -3356,11 +3514,11 @@
     </row>
     <row r="37" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A37" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B37" s="13"/>
       <c r="C37" s="14" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="D37" s="13"/>
       <c r="E37" s="13"/>
@@ -3370,20 +3528,20 @@
       <c r="I37" s="13"/>
       <c r="J37" s="13"/>
       <c r="K37" s="14" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="L37" s="24" t="s">
         <v>21</v>
       </c>
       <c r="M37" s="17" t="s">
-        <v>449</v>
-      </c>
-      <c r="N37" s="33"/>
+        <v>446</v>
+      </c>
+      <c r="N37" s="32"/>
       <c r="O37" s="16" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="P37" s="16" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="Q37" s="16"/>
       <c r="R37" s="16"/>
@@ -3392,11 +3550,11 @@
     </row>
     <row r="38" spans="1:27" ht="32" x14ac:dyDescent="0.2">
       <c r="A38" s="4" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B38" s="13"/>
       <c r="C38" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D38" s="13"/>
       <c r="E38" s="13"/>
@@ -3406,15 +3564,15 @@
       <c r="I38" s="13"/>
       <c r="J38" s="13"/>
       <c r="K38" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="L38" s="15" t="s">
         <v>21</v>
       </c>
       <c r="M38" s="17"/>
-      <c r="N38" s="33"/>
+      <c r="N38" s="32"/>
       <c r="O38" s="16" t="s">
-        <v>470</v>
+        <v>467</v>
       </c>
       <c r="P38" s="16"/>
       <c r="Q38" s="16"/>
@@ -3424,16 +3582,16 @@
     </row>
     <row r="39" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A39" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B39" s="13"/>
       <c r="C39" s="14" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="D39" s="13"/>
       <c r="E39" s="13"/>
       <c r="F39" s="14" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
       <c r="G39" s="13"/>
       <c r="H39" s="13"/>
@@ -3446,9 +3604,9 @@
         <v>21</v>
       </c>
       <c r="M39" s="17" t="s">
-        <v>447</v>
-      </c>
-      <c r="N39" s="33"/>
+        <v>444</v>
+      </c>
+      <c r="N39" s="32"/>
       <c r="O39" s="16"/>
       <c r="P39" s="16"/>
       <c r="Q39" s="16"/>
@@ -3458,31 +3616,31 @@
     </row>
     <row r="40" spans="1:27" ht="32" x14ac:dyDescent="0.2">
       <c r="A40" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B40" s="13"/>
       <c r="C40" s="14" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="D40" s="13"/>
       <c r="E40" s="13"/>
       <c r="F40" s="14" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="G40" s="13"/>
       <c r="H40" s="13"/>
       <c r="I40" s="13"/>
       <c r="J40" s="13"/>
       <c r="K40" s="14" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="L40" s="25" t="s">
         <v>21</v>
       </c>
       <c r="M40" s="17" t="s">
-        <v>447</v>
-      </c>
-      <c r="N40" s="33"/>
+        <v>444</v>
+      </c>
+      <c r="N40" s="32"/>
       <c r="O40" s="16"/>
       <c r="P40" s="16"/>
       <c r="Q40" s="16"/>
@@ -3492,16 +3650,16 @@
     </row>
     <row r="41" spans="1:27" ht="32" x14ac:dyDescent="0.2">
       <c r="A41" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B41" s="13"/>
       <c r="C41" s="14" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="D41" s="13"/>
       <c r="E41" s="13"/>
       <c r="F41" s="14" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="G41" s="13"/>
       <c r="H41" s="13"/>
@@ -3512,9 +3670,9 @@
         <v>21</v>
       </c>
       <c r="M41" s="17" t="s">
-        <v>447</v>
-      </c>
-      <c r="N41" s="33"/>
+        <v>444</v>
+      </c>
+      <c r="N41" s="32"/>
       <c r="O41" s="16"/>
       <c r="P41" s="16"/>
       <c r="Q41" s="16"/>
@@ -3524,23 +3682,23 @@
     </row>
     <row r="42" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A42" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>187</v>
       </c>
-      <c r="D42" s="4" t="s">
+      <c r="E42" s="4" t="s">
         <v>188</v>
       </c>
-      <c r="E42" s="4" t="s">
+      <c r="F42" s="5" t="s">
         <v>189</v>
       </c>
-      <c r="F42" s="5" t="s">
+      <c r="G42" s="4" t="s">
         <v>190</v>
-      </c>
-      <c r="G42" s="4" t="s">
-        <v>191</v>
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="4">
@@ -3548,31 +3706,31 @@
       </c>
       <c r="J42" s="4"/>
       <c r="K42" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L42" s="7"/>
       <c r="M42" s="7"/>
-      <c r="N42" s="29"/>
+      <c r="N42" s="28"/>
     </row>
     <row r="43" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A43" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="D43" s="4" t="s">
         <v>193</v>
       </c>
-      <c r="D43" s="4" t="s">
+      <c r="E43" s="4" t="s">
         <v>194</v>
       </c>
-      <c r="E43" s="4" t="s">
+      <c r="F43" s="5" t="s">
         <v>195</v>
       </c>
-      <c r="F43" s="5" t="s">
-        <v>196</v>
-      </c>
       <c r="G43" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="4">
@@ -3580,31 +3738,31 @@
       </c>
       <c r="J43" s="4"/>
       <c r="K43" s="5" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="L43" s="7"/>
       <c r="M43" s="7"/>
-      <c r="N43" s="29"/>
-    </row>
-    <row r="44" spans="1:27" ht="64" x14ac:dyDescent="0.2">
+      <c r="N43" s="28"/>
+    </row>
+    <row r="44" spans="1:27" ht="112" x14ac:dyDescent="0.2">
       <c r="A44" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="D44" s="4" t="s">
         <v>197</v>
       </c>
-      <c r="D44" s="4" t="s">
+      <c r="E44" s="4" t="s">
         <v>198</v>
       </c>
-      <c r="E44" s="4" t="s">
+      <c r="F44" s="5" t="s">
         <v>199</v>
       </c>
-      <c r="F44" s="5" t="s">
-        <v>200</v>
-      </c>
       <c r="G44" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H44" s="4">
         <v>2015</v>
@@ -3614,15 +3772,23 @@
       </c>
       <c r="J44" s="4"/>
       <c r="K44" s="5" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="L44" s="7" t="s">
         <v>21</v>
       </c>
       <c r="M44" s="8" t="s">
-        <v>202</v>
-      </c>
-      <c r="N44" s="31"/>
+        <v>508</v>
+      </c>
+      <c r="N44" s="30" t="s">
+        <v>505</v>
+      </c>
+      <c r="O44" t="s">
+        <v>506</v>
+      </c>
+      <c r="P44" t="s">
+        <v>507</v>
+      </c>
       <c r="Z44">
         <v>4</v>
       </c>
@@ -3630,25 +3796,25 @@
         <v>0</v>
       </c>
     </row>
-    <row r="45" spans="1:27" ht="80" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:27" ht="192" x14ac:dyDescent="0.2">
       <c r="A45" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E45" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="D45" s="4" t="s">
+      <c r="F45" s="5" t="s">
         <v>204</v>
       </c>
-      <c r="E45" s="4" t="s">
-        <v>205</v>
-      </c>
-      <c r="F45" s="5" t="s">
-        <v>206</v>
-      </c>
       <c r="G45" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H45" s="4">
         <v>1900</v>
@@ -3658,15 +3824,26 @@
       </c>
       <c r="J45" s="4"/>
       <c r="K45" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="L45" s="7" t="s">
         <v>21</v>
       </c>
       <c r="M45" s="8" t="s">
-        <v>208</v>
-      </c>
-      <c r="N45" s="31"/>
+        <v>508</v>
+      </c>
+      <c r="N45" s="30" t="s">
+        <v>509</v>
+      </c>
+      <c r="O45" t="s">
+        <v>515</v>
+      </c>
+      <c r="P45" s="34" t="s">
+        <v>510</v>
+      </c>
+      <c r="U45" s="30" t="s">
+        <v>512</v>
+      </c>
       <c r="Z45">
         <v>4</v>
       </c>
@@ -3676,88 +3853,72 @@
     </row>
     <row r="46" spans="1:27" ht="32" x14ac:dyDescent="0.2">
       <c r="A46" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B46" s="4"/>
       <c r="C46" s="5" t="s">
-        <v>209</v>
-      </c>
-      <c r="D46" s="4" t="s">
-        <v>210</v>
-      </c>
-      <c r="E46" s="4" t="s">
-        <v>211</v>
-      </c>
+        <v>511</v>
+      </c>
+      <c r="D46" s="4"/>
+      <c r="E46" s="4"/>
       <c r="F46" s="5" t="s">
-        <v>212</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>191</v>
-      </c>
-      <c r="H46" s="4"/>
-      <c r="I46" s="4"/>
+        <v>513</v>
+      </c>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4">
+        <v>1992</v>
+      </c>
+      <c r="I46" s="4">
+        <v>2017</v>
+      </c>
       <c r="J46" s="4"/>
-      <c r="K46" s="5" t="s">
-        <v>213</v>
-      </c>
-      <c r="L46" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="M46" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="N46" s="29"/>
-      <c r="O46" t="s">
-        <v>473</v>
-      </c>
-      <c r="P46" t="s">
-        <v>474</v>
-      </c>
-      <c r="Z46">
-        <v>4</v>
-      </c>
-      <c r="AA46" t="b">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="1:27" ht="80" x14ac:dyDescent="0.2">
+      <c r="K46" s="5"/>
+      <c r="L46" s="7"/>
+      <c r="M46" s="8" t="s">
+        <v>508</v>
+      </c>
+      <c r="N46" t="s">
+        <v>514</v>
+      </c>
+    </row>
+    <row r="47" spans="1:27" ht="32" x14ac:dyDescent="0.2">
       <c r="A47" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B47" s="4"/>
       <c r="C47" s="5" t="s">
-        <v>214</v>
+        <v>206</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>215</v>
+        <v>207</v>
       </c>
       <c r="E47" s="4" t="s">
-        <v>216</v>
+        <v>208</v>
       </c>
       <c r="F47" s="5" t="s">
-        <v>217</v>
+        <v>209</v>
       </c>
       <c r="G47" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H47" s="4"/>
       <c r="I47" s="4"/>
       <c r="J47" s="4"/>
       <c r="K47" s="5" t="s">
-        <v>475</v>
+        <v>210</v>
       </c>
       <c r="L47" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="M47" s="8" t="s">
-        <v>477</v>
-      </c>
-      <c r="N47" s="31"/>
+      <c r="M47" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="N47" s="28"/>
       <c r="O47" t="s">
-        <v>478</v>
+        <v>470</v>
       </c>
       <c r="P47" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="Z47">
         <v>4</v>
@@ -3766,39 +3927,45 @@
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:27" ht="32" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:27" ht="80" x14ac:dyDescent="0.2">
       <c r="A48" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="5" t="s">
-        <v>218</v>
+        <v>211</v>
       </c>
       <c r="D48" s="4" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="E48" s="4" t="s">
-        <v>220</v>
+        <v>213</v>
       </c>
       <c r="F48" s="5" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G48" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
       <c r="J48" s="4"/>
-      <c r="K48" s="14" t="s">
-        <v>213</v>
+      <c r="K48" s="5" t="s">
+        <v>472</v>
       </c>
       <c r="L48" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="M48" s="7" t="s">
-        <v>459</v>
-      </c>
-      <c r="N48" s="29"/>
+      <c r="M48" s="8" t="s">
+        <v>474</v>
+      </c>
+      <c r="N48" s="30"/>
+      <c r="O48" t="s">
+        <v>475</v>
+      </c>
+      <c r="P48" t="s">
+        <v>473</v>
+      </c>
       <c r="Z48">
         <v>4</v>
       </c>
@@ -3806,235 +3973,257 @@
         <v>0</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:27" ht="32" x14ac:dyDescent="0.2">
       <c r="A49" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B49" s="4"/>
       <c r="C49" s="5" t="s">
-        <v>457</v>
+        <v>215</v>
       </c>
       <c r="D49" s="4" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E49" s="4" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="F49" s="5" t="s">
-        <v>458</v>
+        <v>218</v>
       </c>
       <c r="G49" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H49" s="4"/>
       <c r="I49" s="4"/>
       <c r="J49" s="4"/>
-      <c r="K49" s="5" t="s">
-        <v>451</v>
+      <c r="K49" s="14" t="s">
+        <v>210</v>
       </c>
       <c r="L49" s="18" t="s">
         <v>21</v>
       </c>
       <c r="M49" s="7" t="s">
-        <v>446</v>
-      </c>
-      <c r="N49" s="29"/>
-    </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+        <v>456</v>
+      </c>
+      <c r="N49" s="28"/>
+      <c r="Z49">
+        <v>4</v>
+      </c>
+      <c r="AA49" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A50" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="5" t="s">
-        <v>479</v>
-      </c>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="5"/>
-      <c r="G50" s="4"/>
+        <v>454</v>
+      </c>
+      <c r="D50" s="4" t="s">
+        <v>219</v>
+      </c>
+      <c r="E50" s="4" t="s">
+        <v>220</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>455</v>
+      </c>
+      <c r="G50" s="4" t="s">
+        <v>190</v>
+      </c>
       <c r="H50" s="4"/>
       <c r="I50" s="4"/>
       <c r="J50" s="4"/>
-      <c r="K50" s="5"/>
-      <c r="L50" s="18"/>
-      <c r="M50" s="7"/>
-      <c r="N50" s="29"/>
-    </row>
-    <row r="51" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="K50" s="5" t="s">
+        <v>448</v>
+      </c>
+      <c r="L50" s="18" t="s">
+        <v>21</v>
+      </c>
+      <c r="M50" s="7" t="s">
+        <v>443</v>
+      </c>
+      <c r="N50" s="28"/>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A51" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="5" t="s">
-        <v>224</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>225</v>
-      </c>
-      <c r="E51" s="4" t="s">
-        <v>226</v>
-      </c>
-      <c r="F51" s="14" t="s">
-        <v>227</v>
-      </c>
-      <c r="G51" s="4" t="s">
-        <v>191</v>
-      </c>
+        <v>476</v>
+      </c>
+      <c r="D51" s="4"/>
+      <c r="E51" s="4"/>
+      <c r="F51" s="5"/>
+      <c r="G51" s="4"/>
       <c r="H51" s="4"/>
       <c r="I51" s="4"/>
       <c r="J51" s="4"/>
-      <c r="K51" s="14" t="s">
-        <v>213</v>
-      </c>
-      <c r="L51" s="7"/>
+      <c r="K51" s="5"/>
+      <c r="L51" s="18"/>
       <c r="M51" s="7"/>
-      <c r="N51" s="29"/>
-    </row>
-    <row r="52" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="N51" s="28"/>
+    </row>
+    <row r="52" spans="1:27" ht="32" x14ac:dyDescent="0.2">
       <c r="A52" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="5" t="s">
-        <v>228</v>
+        <v>221</v>
       </c>
       <c r="D52" s="4" t="s">
-        <v>229</v>
+        <v>222</v>
       </c>
       <c r="E52" s="4" t="s">
-        <v>230</v>
-      </c>
-      <c r="F52" s="5" t="s">
-        <v>231</v>
+        <v>223</v>
+      </c>
+      <c r="F52" s="14" t="s">
+        <v>224</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H52" s="4"/>
       <c r="I52" s="4"/>
       <c r="J52" s="4"/>
       <c r="K52" s="14" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="L52" s="7"/>
       <c r="M52" s="7"/>
-      <c r="N52" s="29"/>
-    </row>
-    <row r="53" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="N52" s="28"/>
+    </row>
+    <row r="53" spans="1:27" ht="32" x14ac:dyDescent="0.2">
       <c r="A53" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B53" s="4"/>
       <c r="C53" s="5" t="s">
-        <v>232</v>
+        <v>225</v>
       </c>
       <c r="D53" s="4" t="s">
-        <v>233</v>
+        <v>226</v>
       </c>
       <c r="E53" s="4" t="s">
-        <v>234</v>
+        <v>227</v>
       </c>
       <c r="F53" s="5" t="s">
-        <v>235</v>
+        <v>228</v>
       </c>
       <c r="G53" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
       <c r="J53" s="4"/>
-      <c r="K53" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="L53" s="7" t="s">
-        <v>21</v>
-      </c>
+      <c r="K53" s="14" t="s">
+        <v>210</v>
+      </c>
+      <c r="L53" s="7"/>
       <c r="M53" s="7"/>
-      <c r="N53" s="29"/>
-    </row>
-    <row r="54" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="N53" s="28"/>
+    </row>
+    <row r="54" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A54" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B54" s="4"/>
       <c r="C54" s="5" t="s">
-        <v>180</v>
+        <v>229</v>
       </c>
       <c r="D54" s="4" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="E54" s="4" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="F54" s="5" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="G54" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
       <c r="J54" s="4"/>
       <c r="K54" s="5" t="s">
-        <v>239</v>
+        <v>20</v>
       </c>
       <c r="L54" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M54" s="7"/>
-      <c r="N54" s="29"/>
-    </row>
-    <row r="55" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="M54" s="7" t="s">
+        <v>516</v>
+      </c>
+      <c r="N54" s="28" t="s">
+        <v>518</v>
+      </c>
+      <c r="O54" s="35" t="s">
+        <v>517</v>
+      </c>
+      <c r="P54" s="35" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="55" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A55" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B55" s="4"/>
       <c r="C55" s="5" t="s">
-        <v>240</v>
+        <v>179</v>
       </c>
       <c r="D55" s="4" t="s">
-        <v>241</v>
+        <v>233</v>
       </c>
       <c r="E55" s="4" t="s">
-        <v>242</v>
+        <v>234</v>
       </c>
       <c r="F55" s="5" t="s">
-        <v>243</v>
+        <v>235</v>
       </c>
       <c r="G55" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H55" s="4"/>
       <c r="I55" s="4"/>
       <c r="J55" s="4"/>
       <c r="K55" s="5" t="s">
-        <v>20</v>
+        <v>236</v>
       </c>
       <c r="L55" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M55" s="7"/>
-      <c r="N55" s="29"/>
-    </row>
-    <row r="56" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+      <c r="M55" s="7" t="s">
+        <v>521</v>
+      </c>
+      <c r="N55" s="28" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="56" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A56" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B56" s="4"/>
       <c r="C56" s="5" t="s">
-        <v>244</v>
+        <v>237</v>
       </c>
       <c r="D56" s="4" t="s">
-        <v>245</v>
+        <v>238</v>
       </c>
       <c r="E56" s="4" t="s">
-        <v>246</v>
+        <v>239</v>
       </c>
       <c r="F56" s="5" t="s">
-        <v>247</v>
+        <v>240</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
@@ -4045,28 +4234,32 @@
       <c r="L56" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M56" s="7"/>
-      <c r="N56" s="29"/>
-    </row>
-    <row r="57" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="M56" s="7" t="s">
+        <v>523</v>
+      </c>
+      <c r="N56" s="28" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="57" spans="1:27" ht="64" x14ac:dyDescent="0.2">
       <c r="A57" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B57" s="4"/>
       <c r="C57" s="5" t="s">
-        <v>248</v>
+        <v>241</v>
       </c>
       <c r="D57" s="4" t="s">
-        <v>249</v>
+        <v>242</v>
       </c>
       <c r="E57" s="4" t="s">
-        <v>250</v>
+        <v>243</v>
       </c>
       <c r="F57" s="5" t="s">
-        <v>251</v>
+        <v>244</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
@@ -4077,28 +4270,32 @@
       <c r="L57" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M57" s="7"/>
-      <c r="N57" s="29"/>
-    </row>
-    <row r="58" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="M57" s="7" t="s">
+        <v>527</v>
+      </c>
+      <c r="N57" s="35" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="58" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A58" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B58" s="4"/>
       <c r="C58" s="5" t="s">
-        <v>252</v>
+        <v>245</v>
       </c>
       <c r="D58" s="4" t="s">
-        <v>253</v>
+        <v>246</v>
       </c>
       <c r="E58" s="4" t="s">
-        <v>254</v>
+        <v>247</v>
       </c>
       <c r="F58" s="5" t="s">
-        <v>255</v>
+        <v>248</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H58" s="4"/>
       <c r="I58" s="4"/>
@@ -4109,28 +4306,30 @@
       <c r="L58" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M58" s="7"/>
-      <c r="N58" s="29"/>
-    </row>
-    <row r="59" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="M58" s="7" t="s">
+        <v>524</v>
+      </c>
+      <c r="N58" s="28"/>
+    </row>
+    <row r="59" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A59" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B59" s="4"/>
       <c r="C59" s="5" t="s">
-        <v>256</v>
+        <v>249</v>
       </c>
       <c r="D59" s="4" t="s">
-        <v>257</v>
+        <v>250</v>
       </c>
       <c r="E59" s="4" t="s">
-        <v>258</v>
+        <v>251</v>
       </c>
       <c r="F59" s="5" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
@@ -4138,97 +4337,113 @@
       <c r="K59" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="L59" s="22" t="s">
+      <c r="L59" s="7" t="s">
         <v>21</v>
       </c>
       <c r="M59" s="7" t="s">
-        <v>447</v>
-      </c>
-      <c r="N59" s="29"/>
-    </row>
-    <row r="60" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>527</v>
+      </c>
+      <c r="N59" s="35" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="60" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A60" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B60" s="4"/>
       <c r="C60" s="5" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="D60" s="4" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
       <c r="E60" s="4" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
       <c r="F60" s="5" t="s">
-        <v>263</v>
+        <v>256</v>
       </c>
       <c r="G60" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
       <c r="J60" s="4"/>
       <c r="K60" s="5" t="s">
-        <v>264</v>
-      </c>
-      <c r="L60" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="L60" s="36" t="s">
         <v>21</v>
       </c>
-      <c r="M60" s="7"/>
-      <c r="N60" s="29"/>
-    </row>
-    <row r="61" spans="1:14" ht="128" x14ac:dyDescent="0.2">
+      <c r="M60" s="7" t="s">
+        <v>530</v>
+      </c>
+      <c r="N60" s="35" t="s">
+        <v>528</v>
+      </c>
+      <c r="O60" s="7" t="s">
+        <v>529</v>
+      </c>
+      <c r="P60" s="35" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="61" spans="1:27" ht="32" x14ac:dyDescent="0.2">
       <c r="A61" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B61" s="4"/>
       <c r="C61" s="5" t="s">
-        <v>265</v>
+        <v>257</v>
       </c>
       <c r="D61" s="4" t="s">
-        <v>266</v>
+        <v>258</v>
       </c>
       <c r="E61" s="4" t="s">
-        <v>267</v>
+        <v>259</v>
       </c>
       <c r="F61" s="5" t="s">
-        <v>268</v>
+        <v>260</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
       <c r="J61" s="4"/>
       <c r="K61" s="5" t="s">
-        <v>20</v>
+        <v>261</v>
       </c>
       <c r="L61" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M61" s="7"/>
-      <c r="N61" s="29"/>
-    </row>
-    <row r="62" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+      <c r="M61" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="N61" s="35" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="62" spans="1:27" ht="128" x14ac:dyDescent="0.2">
       <c r="A62" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B62" s="4"/>
       <c r="C62" s="5" t="s">
-        <v>269</v>
+        <v>262</v>
       </c>
       <c r="D62" s="4" t="s">
-        <v>270</v>
+        <v>263</v>
       </c>
       <c r="E62" s="4" t="s">
-        <v>271</v>
+        <v>264</v>
       </c>
       <c r="F62" s="5" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H62" s="4"/>
       <c r="I62" s="4"/>
@@ -4239,28 +4454,32 @@
       <c r="L62" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M62" s="7"/>
-      <c r="N62" s="29"/>
-    </row>
-    <row r="63" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="M62" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="N62" s="35" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="63" spans="1:27" ht="64" x14ac:dyDescent="0.2">
       <c r="A63" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B63" s="4"/>
       <c r="C63" s="5" t="s">
-        <v>273</v>
+        <v>266</v>
       </c>
       <c r="D63" s="4" t="s">
-        <v>274</v>
+        <v>267</v>
       </c>
       <c r="E63" s="4" t="s">
-        <v>275</v>
+        <v>268</v>
       </c>
       <c r="F63" s="5" t="s">
-        <v>276</v>
+        <v>269</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
@@ -4271,92 +4490,107 @@
       <c r="L63" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M63" s="7"/>
-      <c r="N63" s="29"/>
-    </row>
-    <row r="64" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="M63" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="N63" s="35" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="64" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A64" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B64" s="4"/>
       <c r="C64" s="5" t="s">
-        <v>277</v>
+        <v>270</v>
       </c>
       <c r="D64" s="4" t="s">
-        <v>278</v>
+        <v>271</v>
       </c>
       <c r="E64" s="4" t="s">
-        <v>279</v>
+        <v>272</v>
       </c>
       <c r="F64" s="5" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="G64" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
       <c r="K64" s="5" t="s">
-        <v>239</v>
+        <v>20</v>
       </c>
       <c r="L64" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M64" s="7"/>
-      <c r="N64" s="29"/>
-    </row>
-    <row r="65" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="M64" s="7" t="s">
+        <v>533</v>
+      </c>
+      <c r="N64" s="35" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="65" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A65" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B65" s="4"/>
       <c r="C65" s="5" t="s">
-        <v>281</v>
+        <v>274</v>
       </c>
       <c r="D65" s="4" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
       <c r="E65" s="4" t="s">
-        <v>283</v>
+        <v>276</v>
       </c>
       <c r="F65" s="5" t="s">
-        <v>284</v>
+        <v>277</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
       <c r="J65" s="4"/>
       <c r="K65" s="5" t="s">
-        <v>20</v>
+        <v>236</v>
       </c>
       <c r="L65" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M65" s="7"/>
-      <c r="N65" s="29"/>
-    </row>
-    <row r="66" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="M65" s="7" t="s">
+        <v>537</v>
+      </c>
+      <c r="N65" s="35" t="s">
+        <v>536</v>
+      </c>
+      <c r="O65" s="35" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="66" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A66" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B66" s="4"/>
       <c r="C66" s="5" t="s">
-        <v>285</v>
+        <v>278</v>
       </c>
       <c r="D66" s="4" t="s">
-        <v>286</v>
+        <v>279</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>287</v>
+        <v>280</v>
       </c>
       <c r="F66" s="5" t="s">
-        <v>288</v>
+        <v>281</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
@@ -4367,28 +4601,41 @@
       <c r="L66" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M66" s="7"/>
-      <c r="N66" s="29"/>
-    </row>
-    <row r="67" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+      <c r="M66" s="7" t="s">
+        <v>541</v>
+      </c>
+      <c r="N66" s="35" t="s">
+        <v>539</v>
+      </c>
+      <c r="O66" s="35" t="s">
+        <v>540</v>
+      </c>
+      <c r="P66" s="35" t="s">
+        <v>542</v>
+      </c>
+      <c r="Q66" s="35" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="67" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A67" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B67" s="4"/>
       <c r="C67" s="5" t="s">
-        <v>289</v>
+        <v>282</v>
       </c>
       <c r="D67" s="4" t="s">
-        <v>290</v>
+        <v>283</v>
       </c>
       <c r="E67" s="4" t="s">
-        <v>291</v>
+        <v>284</v>
       </c>
       <c r="F67" s="5" t="s">
-        <v>292</v>
+        <v>285</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
@@ -4400,155 +4647,166 @@
         <v>21</v>
       </c>
       <c r="M67" s="7"/>
-      <c r="N67" s="29"/>
-    </row>
-    <row r="68" spans="1:14" ht="112" x14ac:dyDescent="0.2">
+      <c r="N67" s="35" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="68" spans="1:17" ht="80" x14ac:dyDescent="0.2">
       <c r="A68" s="4" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B68" s="4"/>
       <c r="C68" s="5" t="s">
-        <v>293</v>
+        <v>286</v>
       </c>
       <c r="D68" s="4" t="s">
-        <v>204</v>
+        <v>287</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>294</v>
+        <v>288</v>
       </c>
       <c r="F68" s="5" t="s">
-        <v>295</v>
+        <v>289</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="H68" s="4"/>
       <c r="I68" s="4"/>
       <c r="J68" s="4"/>
       <c r="K68" s="5" t="s">
-        <v>296</v>
+        <v>20</v>
       </c>
       <c r="L68" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M68" s="8" t="s">
-        <v>461</v>
-      </c>
-      <c r="N68" s="31"/>
-    </row>
-    <row r="69" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="M68" s="7" t="s">
+        <v>546</v>
+      </c>
+      <c r="N68" s="35" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="69" spans="1:17" ht="112" x14ac:dyDescent="0.2">
       <c r="A69" s="4" t="s">
-        <v>297</v>
+        <v>185</v>
       </c>
       <c r="B69" s="4"/>
       <c r="C69" s="5" t="s">
-        <v>298</v>
+        <v>290</v>
       </c>
       <c r="D69" s="4" t="s">
-        <v>299</v>
+        <v>202</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="F69" s="5" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>302</v>
+        <v>190</v>
       </c>
       <c r="H69" s="4"/>
-      <c r="I69" s="4">
-        <v>2011</v>
-      </c>
+      <c r="I69" s="4"/>
       <c r="J69" s="4"/>
       <c r="K69" s="5" t="s">
-        <v>303</v>
-      </c>
-      <c r="L69" s="7"/>
-      <c r="M69" s="7"/>
-      <c r="N69" s="29"/>
-    </row>
-    <row r="70" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+        <v>293</v>
+      </c>
+      <c r="L69" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M69" s="8" t="s">
+        <v>458</v>
+      </c>
+      <c r="N69" s="30" t="s">
+        <v>547</v>
+      </c>
+      <c r="O69" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="70" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A70" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B70" s="4"/>
       <c r="C70" s="5" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="D70" s="4" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="E70" s="4" t="s">
-        <v>305</v>
+        <v>297</v>
       </c>
       <c r="F70" s="5" t="s">
-        <v>306</v>
+        <v>298</v>
       </c>
       <c r="G70" s="4" t="s">
-        <v>307</v>
+        <v>299</v>
       </c>
       <c r="H70" s="4"/>
-      <c r="I70" s="4"/>
+      <c r="I70" s="4">
+        <v>2011</v>
+      </c>
       <c r="J70" s="4"/>
       <c r="K70" s="5" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="L70" s="7"/>
       <c r="M70" s="7"/>
-      <c r="N70" s="29"/>
-    </row>
-    <row r="71" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="N70" s="28"/>
+    </row>
+    <row r="71" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A71" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B71" s="4"/>
       <c r="C71" s="5" t="s">
-        <v>309</v>
+        <v>301</v>
       </c>
       <c r="D71" s="4" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="E71" s="4" t="s">
-        <v>310</v>
+        <v>302</v>
       </c>
       <c r="F71" s="5" t="s">
-        <v>311</v>
+        <v>303</v>
       </c>
       <c r="G71" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H71" s="4"/>
-      <c r="I71" s="4">
-        <v>2014</v>
-      </c>
+      <c r="I71" s="4"/>
       <c r="J71" s="4"/>
       <c r="K71" s="5" t="s">
-        <v>312</v>
+        <v>305</v>
       </c>
       <c r="L71" s="7"/>
       <c r="M71" s="7"/>
-      <c r="N71" s="29"/>
-    </row>
-    <row r="72" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="N71" s="28"/>
+    </row>
+    <row r="72" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A72" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B72" s="4"/>
       <c r="C72" s="5" t="s">
-        <v>313</v>
+        <v>306</v>
       </c>
       <c r="D72" s="4" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="E72" s="4" t="s">
-        <v>314</v>
+        <v>307</v>
       </c>
       <c r="F72" s="5" t="s">
-        <v>315</v>
+        <v>308</v>
       </c>
       <c r="G72" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H72" s="4"/>
       <c r="I72" s="4">
@@ -4556,921 +4814,914 @@
       </c>
       <c r="J72" s="4"/>
       <c r="K72" s="5" t="s">
-        <v>312</v>
+        <v>309</v>
       </c>
       <c r="L72" s="7"/>
       <c r="M72" s="7"/>
-      <c r="N72" s="29"/>
-    </row>
-    <row r="73" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="N72" s="28"/>
+    </row>
+    <row r="73" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A73" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B73" s="4"/>
       <c r="C73" s="5" t="s">
-        <v>316</v>
+        <v>310</v>
       </c>
       <c r="D73" s="4" t="s">
-        <v>317</v>
+        <v>311</v>
       </c>
       <c r="E73" s="4" t="s">
-        <v>318</v>
+        <v>311</v>
       </c>
       <c r="F73" s="5" t="s">
-        <v>319</v>
+        <v>312</v>
       </c>
       <c r="G73" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H73" s="4"/>
       <c r="I73" s="4">
-        <v>2015</v>
+        <v>2014</v>
       </c>
       <c r="J73" s="4"/>
       <c r="K73" s="5" t="s">
-        <v>320</v>
+        <v>309</v>
       </c>
       <c r="L73" s="7"/>
       <c r="M73" s="7"/>
-      <c r="N73" s="29"/>
-    </row>
-    <row r="74" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="N73" s="28"/>
+    </row>
+    <row r="74" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A74" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B74" s="4"/>
       <c r="C74" s="5" t="s">
-        <v>321</v>
+        <v>313</v>
       </c>
       <c r="D74" s="4" t="s">
-        <v>322</v>
+        <v>314</v>
       </c>
       <c r="E74" s="4" t="s">
-        <v>323</v>
+        <v>315</v>
       </c>
       <c r="F74" s="5" t="s">
-        <v>324</v>
+        <v>316</v>
       </c>
       <c r="G74" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H74" s="4"/>
-      <c r="I74" s="4"/>
+      <c r="I74" s="4">
+        <v>2015</v>
+      </c>
       <c r="J74" s="4"/>
       <c r="K74" s="5" t="s">
-        <v>325</v>
+        <v>317</v>
       </c>
       <c r="L74" s="7"/>
       <c r="M74" s="7"/>
-      <c r="N74" s="29"/>
-    </row>
-    <row r="75" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="N74" s="28"/>
+    </row>
+    <row r="75" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A75" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B75" s="4"/>
       <c r="C75" s="5" t="s">
-        <v>326</v>
+        <v>318</v>
       </c>
       <c r="D75" s="4" t="s">
-        <v>327</v>
+        <v>319</v>
       </c>
       <c r="E75" s="4" t="s">
-        <v>328</v>
+        <v>320</v>
       </c>
       <c r="F75" s="5" t="s">
-        <v>329</v>
+        <v>321</v>
       </c>
       <c r="G75" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
       <c r="J75" s="4"/>
       <c r="K75" s="5" t="s">
-        <v>330</v>
+        <v>322</v>
       </c>
       <c r="L75" s="7"/>
       <c r="M75" s="7"/>
-      <c r="N75" s="29"/>
-    </row>
-    <row r="76" spans="1:14" ht="32" x14ac:dyDescent="0.2">
+      <c r="N75" s="28"/>
+    </row>
+    <row r="76" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A76" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B76" s="4"/>
       <c r="C76" s="5" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="D76" s="4" t="s">
-        <v>332</v>
+        <v>324</v>
       </c>
       <c r="E76" s="4" t="s">
-        <v>333</v>
+        <v>325</v>
       </c>
       <c r="F76" s="5" t="s">
-        <v>334</v>
+        <v>326</v>
       </c>
       <c r="G76" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
       <c r="J76" s="4"/>
       <c r="K76" s="5" t="s">
-        <v>335</v>
+        <v>327</v>
       </c>
       <c r="L76" s="7"/>
       <c r="M76" s="7"/>
-      <c r="N76" s="29"/>
-    </row>
-    <row r="77" spans="1:14" ht="80" x14ac:dyDescent="0.2">
+      <c r="N76" s="28"/>
+    </row>
+    <row r="77" spans="1:17" ht="32" x14ac:dyDescent="0.2">
       <c r="A77" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B77" s="4"/>
       <c r="C77" s="5" t="s">
-        <v>336</v>
+        <v>328</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>337</v>
+        <v>329</v>
       </c>
       <c r="E77" s="4" t="s">
-        <v>338</v>
+        <v>330</v>
       </c>
       <c r="F77" s="5" t="s">
-        <v>339</v>
+        <v>331</v>
       </c>
       <c r="G77" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
       <c r="J77" s="4"/>
       <c r="K77" s="5" t="s">
-        <v>340</v>
+        <v>332</v>
       </c>
       <c r="L77" s="7"/>
       <c r="M77" s="7"/>
-      <c r="N77" s="29"/>
-    </row>
-    <row r="78" spans="1:14" ht="48" x14ac:dyDescent="0.2">
+      <c r="N77" s="28"/>
+    </row>
+    <row r="78" spans="1:17" ht="80" x14ac:dyDescent="0.2">
       <c r="A78" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B78" s="4"/>
       <c r="C78" s="5" t="s">
-        <v>341</v>
+        <v>333</v>
       </c>
       <c r="D78" s="4" t="s">
-        <v>342</v>
+        <v>334</v>
       </c>
       <c r="E78" s="4" t="s">
-        <v>343</v>
+        <v>335</v>
       </c>
       <c r="F78" s="5" t="s">
-        <v>344</v>
+        <v>336</v>
       </c>
       <c r="G78" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
       <c r="J78" s="4"/>
       <c r="K78" s="5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="L78" s="7"/>
       <c r="M78" s="7"/>
-      <c r="N78" s="29"/>
-    </row>
-    <row r="79" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+      <c r="N78" s="28"/>
+    </row>
+    <row r="79" spans="1:17" ht="48" x14ac:dyDescent="0.2">
       <c r="A79" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B79" s="4"/>
       <c r="C79" s="5" t="s">
-        <v>345</v>
+        <v>338</v>
       </c>
       <c r="D79" s="4" t="s">
-        <v>346</v>
+        <v>339</v>
       </c>
       <c r="E79" s="4" t="s">
-        <v>347</v>
+        <v>340</v>
       </c>
       <c r="F79" s="5" t="s">
-        <v>348</v>
+        <v>341</v>
       </c>
       <c r="G79" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
       <c r="J79" s="4"/>
       <c r="K79" s="5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="L79" s="7"/>
       <c r="M79" s="7"/>
-      <c r="N79" s="29"/>
-    </row>
-    <row r="80" spans="1:14" ht="64" x14ac:dyDescent="0.2">
+      <c r="N79" s="28"/>
+    </row>
+    <row r="80" spans="1:17" ht="64" x14ac:dyDescent="0.2">
       <c r="A80" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B80" s="4"/>
       <c r="C80" s="5" t="s">
-        <v>349</v>
+        <v>342</v>
       </c>
       <c r="D80" s="4" t="s">
-        <v>350</v>
+        <v>343</v>
       </c>
       <c r="E80" s="4" t="s">
-        <v>351</v>
+        <v>344</v>
       </c>
       <c r="F80" s="5" t="s">
-        <v>352</v>
+        <v>345</v>
       </c>
       <c r="G80" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
       <c r="J80" s="4"/>
       <c r="K80" s="5" t="s">
-        <v>353</v>
+        <v>337</v>
       </c>
       <c r="L80" s="7"/>
       <c r="M80" s="7"/>
-      <c r="N80" s="29"/>
-    </row>
-    <row r="81" spans="1:27" ht="48" x14ac:dyDescent="0.2">
+      <c r="N80" s="28"/>
+    </row>
+    <row r="81" spans="1:27" ht="64" x14ac:dyDescent="0.2">
       <c r="A81" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B81" s="4"/>
       <c r="C81" s="5" t="s">
-        <v>354</v>
+        <v>346</v>
       </c>
       <c r="D81" s="4" t="s">
-        <v>355</v>
+        <v>347</v>
       </c>
       <c r="E81" s="4" t="s">
-        <v>356</v>
+        <v>348</v>
       </c>
       <c r="F81" s="5" t="s">
-        <v>357</v>
+        <v>349</v>
       </c>
       <c r="G81" s="4" t="s">
-        <v>307</v>
+        <v>304</v>
       </c>
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
       <c r="J81" s="4"/>
       <c r="K81" s="5" t="s">
-        <v>340</v>
+        <v>350</v>
       </c>
       <c r="L81" s="7"/>
       <c r="M81" s="7"/>
-      <c r="N81" s="29"/>
-    </row>
-    <row r="82" spans="1:27" ht="64" x14ac:dyDescent="0.2">
+      <c r="N81" s="28"/>
+    </row>
+    <row r="82" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A82" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B82" s="4"/>
       <c r="C82" s="5" t="s">
-        <v>358</v>
+        <v>351</v>
       </c>
       <c r="D82" s="4" t="s">
-        <v>359</v>
+        <v>352</v>
       </c>
       <c r="E82" s="4" t="s">
-        <v>360</v>
+        <v>353</v>
       </c>
       <c r="F82" s="5" t="s">
-        <v>361</v>
-      </c>
-      <c r="G82" s="4"/>
+        <v>354</v>
+      </c>
+      <c r="G82" s="4" t="s">
+        <v>304</v>
+      </c>
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
       <c r="J82" s="4"/>
       <c r="K82" s="5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="L82" s="7"/>
       <c r="M82" s="7"/>
-      <c r="N82" s="29"/>
-      <c r="T82" s="19"/>
-    </row>
-    <row r="83" spans="1:27" ht="48" x14ac:dyDescent="0.2">
+      <c r="N82" s="28"/>
+    </row>
+    <row r="83" spans="1:27" ht="64" x14ac:dyDescent="0.2">
       <c r="A83" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B83" s="4"/>
       <c r="C83" s="5" t="s">
-        <v>362</v>
+        <v>355</v>
       </c>
       <c r="D83" s="4" t="s">
-        <v>363</v>
+        <v>356</v>
       </c>
       <c r="E83" s="4" t="s">
-        <v>364</v>
+        <v>357</v>
       </c>
       <c r="F83" s="5" t="s">
-        <v>365</v>
+        <v>358</v>
       </c>
       <c r="G83" s="4"/>
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
       <c r="J83" s="4"/>
       <c r="K83" s="5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="L83" s="7"/>
       <c r="M83" s="7"/>
-      <c r="N83" s="29"/>
+      <c r="N83" s="28"/>
+      <c r="T83" s="19"/>
     </row>
     <row r="84" spans="1:27" ht="48" x14ac:dyDescent="0.2">
-      <c r="A84" s="6" t="s">
-        <v>297</v>
-      </c>
-      <c r="B84" s="6"/>
-      <c r="C84" s="10" t="s">
-        <v>366</v>
-      </c>
-      <c r="D84" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="E84" s="6" t="s">
-        <v>368</v>
-      </c>
-      <c r="F84" s="10" t="s">
-        <v>369</v>
-      </c>
-      <c r="G84" s="6"/>
-      <c r="H84" s="6"/>
-      <c r="I84" s="6"/>
-      <c r="J84" s="6"/>
+      <c r="A84" s="4" t="s">
+        <v>294</v>
+      </c>
+      <c r="B84" s="4"/>
+      <c r="C84" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="D84" s="4" t="s">
+        <v>360</v>
+      </c>
+      <c r="E84" s="4" t="s">
+        <v>361</v>
+      </c>
+      <c r="F84" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="G84" s="4"/>
+      <c r="H84" s="4"/>
+      <c r="I84" s="4"/>
+      <c r="J84" s="4"/>
       <c r="K84" s="5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="L84" s="7"/>
       <c r="M84" s="7"/>
-      <c r="N84" s="29"/>
+      <c r="N84" s="28"/>
     </row>
     <row r="85" spans="1:27" ht="48" x14ac:dyDescent="0.2">
-      <c r="A85" s="4" t="s">
-        <v>297</v>
-      </c>
-      <c r="B85" s="4"/>
-      <c r="C85" s="5" t="s">
-        <v>370</v>
-      </c>
-      <c r="D85" s="4" t="s">
-        <v>371</v>
-      </c>
-      <c r="E85" s="4" t="s">
-        <v>372</v>
-      </c>
-      <c r="F85" s="5" t="s">
-        <v>373</v>
-      </c>
-      <c r="G85" s="4"/>
-      <c r="H85" s="4"/>
-      <c r="I85" s="4"/>
-      <c r="J85" s="4"/>
+      <c r="A85" s="6" t="s">
+        <v>294</v>
+      </c>
+      <c r="B85" s="6"/>
+      <c r="C85" s="10" t="s">
+        <v>363</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>364</v>
+      </c>
+      <c r="E85" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="F85" s="10" t="s">
+        <v>366</v>
+      </c>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
       <c r="K85" s="5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="L85" s="7"/>
       <c r="M85" s="7"/>
-      <c r="N85" s="29"/>
+      <c r="N85" s="28"/>
     </row>
     <row r="86" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A86" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B86" s="4"/>
       <c r="C86" s="5" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="D86" s="4" t="s">
-        <v>375</v>
+        <v>368</v>
       </c>
       <c r="E86" s="4" t="s">
-        <v>376</v>
+        <v>369</v>
       </c>
       <c r="F86" s="5" t="s">
-        <v>377</v>
+        <v>370</v>
       </c>
       <c r="G86" s="4"/>
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
       <c r="J86" s="4"/>
       <c r="K86" s="5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="L86" s="7"/>
       <c r="M86" s="7"/>
-      <c r="N86" s="29"/>
+      <c r="N86" s="28"/>
     </row>
     <row r="87" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A87" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B87" s="4"/>
       <c r="C87" s="5" t="s">
-        <v>378</v>
+        <v>371</v>
       </c>
       <c r="D87" s="4" t="s">
-        <v>379</v>
+        <v>372</v>
       </c>
       <c r="E87" s="4" t="s">
-        <v>380</v>
+        <v>373</v>
       </c>
       <c r="F87" s="5" t="s">
-        <v>381</v>
+        <v>374</v>
       </c>
       <c r="G87" s="4"/>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
       <c r="J87" s="4"/>
       <c r="K87" s="5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="L87" s="7"/>
-      <c r="M87" s="8"/>
-      <c r="N87" s="31"/>
+      <c r="M87" s="7"/>
+      <c r="N87" s="28"/>
     </row>
     <row r="88" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A88" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B88" s="4"/>
       <c r="C88" s="5" t="s">
-        <v>382</v>
+        <v>375</v>
       </c>
       <c r="D88" s="4" t="s">
-        <v>383</v>
+        <v>376</v>
       </c>
       <c r="E88" s="4" t="s">
-        <v>384</v>
+        <v>377</v>
       </c>
       <c r="F88" s="5" t="s">
-        <v>385</v>
+        <v>378</v>
       </c>
       <c r="G88" s="4"/>
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
       <c r="J88" s="4"/>
       <c r="K88" s="5" t="s">
-        <v>340</v>
+        <v>337</v>
       </c>
       <c r="L88" s="7"/>
-      <c r="M88" s="7"/>
-      <c r="N88" s="29"/>
-    </row>
-    <row r="89" spans="1:27" ht="64" x14ac:dyDescent="0.2">
+      <c r="M88" s="8"/>
+      <c r="N88" s="30"/>
+    </row>
+    <row r="89" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A89" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B89" s="4"/>
       <c r="C89" s="5" t="s">
-        <v>386</v>
+        <v>379</v>
       </c>
       <c r="D89" s="4" t="s">
-        <v>387</v>
+        <v>380</v>
       </c>
       <c r="E89" s="4" t="s">
-        <v>388</v>
+        <v>381</v>
       </c>
       <c r="F89" s="5" t="s">
-        <v>389</v>
+        <v>382</v>
       </c>
       <c r="G89" s="4"/>
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
       <c r="J89" s="4"/>
       <c r="K89" s="5" t="s">
-        <v>390</v>
+        <v>337</v>
       </c>
       <c r="L89" s="7"/>
       <c r="M89" s="7"/>
-      <c r="N89" s="29"/>
-    </row>
-    <row r="90" spans="1:27" s="12" customFormat="1" ht="64" x14ac:dyDescent="0.2">
+      <c r="N89" s="28"/>
+    </row>
+    <row r="90" spans="1:27" ht="64" x14ac:dyDescent="0.2">
       <c r="A90" s="4" t="s">
-        <v>297</v>
+        <v>294</v>
       </c>
       <c r="B90" s="4"/>
       <c r="C90" s="5" t="s">
-        <v>391</v>
+        <v>383</v>
       </c>
       <c r="D90" s="4" t="s">
-        <v>392</v>
+        <v>384</v>
       </c>
       <c r="E90" s="4" t="s">
-        <v>393</v>
+        <v>385</v>
       </c>
       <c r="F90" s="5" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="G90" s="4"/>
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
       <c r="J90" s="4"/>
       <c r="K90" s="5" t="s">
-        <v>394</v>
-      </c>
-      <c r="L90" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="M90" s="8" t="s">
-        <v>395</v>
-      </c>
-      <c r="N90" s="31"/>
-      <c r="O90"/>
-      <c r="P90"/>
-      <c r="Q90"/>
-      <c r="R90"/>
-      <c r="S90"/>
-      <c r="T90"/>
-      <c r="U90"/>
-      <c r="V90"/>
-      <c r="W90"/>
-      <c r="X90"/>
-      <c r="Y90"/>
-      <c r="Z90"/>
-      <c r="AA90"/>
-    </row>
-    <row r="91" spans="1:27" ht="32" x14ac:dyDescent="0.2">
+        <v>387</v>
+      </c>
+      <c r="L90" s="7"/>
+      <c r="M90" s="7"/>
+      <c r="N90" s="28"/>
+    </row>
+    <row r="91" spans="1:27" s="12" customFormat="1" ht="64" x14ac:dyDescent="0.2">
       <c r="A91" s="4" t="s">
-        <v>396</v>
+        <v>294</v>
       </c>
       <c r="B91" s="4"/>
-      <c r="C91" s="14" t="s">
-        <v>397</v>
+      <c r="C91" s="5" t="s">
+        <v>388</v>
       </c>
       <c r="D91" s="4" t="s">
-        <v>398</v>
+        <v>389</v>
       </c>
       <c r="E91" s="4" t="s">
-        <v>399</v>
+        <v>390</v>
       </c>
       <c r="F91" s="5" t="s">
-        <v>400</v>
+        <v>388</v>
       </c>
       <c r="G91" s="4"/>
       <c r="H91" s="4"/>
-      <c r="I91" s="4">
-        <v>1983</v>
-      </c>
+      <c r="I91" s="4"/>
       <c r="J91" s="4"/>
       <c r="K91" s="5" t="s">
-        <v>401</v>
+        <v>391</v>
       </c>
       <c r="L91" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M91" s="7"/>
-      <c r="N91" s="29"/>
+      <c r="M91" s="8" t="s">
+        <v>392</v>
+      </c>
+      <c r="N91" s="30"/>
+      <c r="O91"/>
+      <c r="P91"/>
+      <c r="Q91"/>
+      <c r="R91"/>
+      <c r="S91"/>
+      <c r="T91"/>
+      <c r="U91"/>
+      <c r="V91"/>
+      <c r="W91"/>
+      <c r="X91"/>
+      <c r="Y91"/>
+      <c r="Z91"/>
+      <c r="AA91"/>
     </row>
     <row r="92" spans="1:27" ht="32" x14ac:dyDescent="0.2">
       <c r="A92" s="4" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B92" s="4"/>
       <c r="C92" s="14" t="s">
-        <v>402</v>
+        <v>394</v>
       </c>
       <c r="D92" s="4" t="s">
-        <v>403</v>
+        <v>395</v>
       </c>
       <c r="E92" s="4" t="s">
-        <v>404</v>
+        <v>396</v>
       </c>
       <c r="F92" s="5" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="G92" s="4"/>
-      <c r="H92" s="13">
-        <v>2013</v>
-      </c>
-      <c r="I92" s="13">
-        <v>2015</v>
+      <c r="H92" s="4"/>
+      <c r="I92" s="4">
+        <v>1983</v>
       </c>
       <c r="J92" s="4"/>
-      <c r="K92" s="14" t="s">
-        <v>406</v>
+      <c r="K92" s="5" t="s">
+        <v>398</v>
       </c>
       <c r="L92" s="7" t="s">
         <v>21</v>
       </c>
       <c r="M92" s="7"/>
-      <c r="N92" s="29"/>
-    </row>
-    <row r="93" spans="1:27" ht="48" x14ac:dyDescent="0.2">
+      <c r="N92" s="28"/>
+    </row>
+    <row r="93" spans="1:27" ht="32" x14ac:dyDescent="0.2">
       <c r="A93" s="4" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B93" s="4"/>
       <c r="C93" s="14" t="s">
-        <v>407</v>
+        <v>399</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>408</v>
-      </c>
-      <c r="E93" s="4"/>
+        <v>400</v>
+      </c>
+      <c r="E93" s="4" t="s">
+        <v>401</v>
+      </c>
       <c r="F93" s="5" t="s">
-        <v>409</v>
+        <v>402</v>
       </c>
       <c r="G93" s="4"/>
-      <c r="H93" s="13"/>
-      <c r="I93" s="13"/>
-      <c r="J93" s="4" t="s">
-        <v>410</v>
-      </c>
+      <c r="H93" s="13">
+        <v>2013</v>
+      </c>
+      <c r="I93" s="13">
+        <v>2015</v>
+      </c>
+      <c r="J93" s="4"/>
       <c r="K93" s="14" t="s">
-        <v>411</v>
+        <v>403</v>
       </c>
       <c r="L93" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M93" s="8" t="s">
-        <v>462</v>
-      </c>
-      <c r="N93" s="31"/>
-    </row>
-    <row r="94" spans="1:27" ht="32" x14ac:dyDescent="0.2">
+      <c r="M93" s="7"/>
+      <c r="N93" s="28"/>
+    </row>
+    <row r="94" spans="1:27" ht="48" x14ac:dyDescent="0.2">
       <c r="A94" s="4" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B94" s="4"/>
       <c r="C94" s="14" t="s">
-        <v>28</v>
+        <v>404</v>
       </c>
       <c r="D94" s="4" t="s">
-        <v>412</v>
-      </c>
-      <c r="E94" s="4" t="s">
-        <v>413</v>
-      </c>
+        <v>405</v>
+      </c>
+      <c r="E94" s="4"/>
       <c r="F94" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="G94" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H94" s="4">
-        <v>2000</v>
-      </c>
-      <c r="I94" s="4">
-        <v>2015</v>
-      </c>
+        <v>406</v>
+      </c>
+      <c r="G94" s="4"/>
+      <c r="H94" s="13"/>
+      <c r="I94" s="13"/>
       <c r="J94" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="K94" s="8" t="s">
-        <v>27</v>
+        <v>407</v>
+      </c>
+      <c r="K94" s="14" t="s">
+        <v>408</v>
       </c>
       <c r="L94" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M94" s="7" t="s">
-        <v>414</v>
-      </c>
-      <c r="N94" s="29"/>
+      <c r="M94" s="8" t="s">
+        <v>459</v>
+      </c>
+      <c r="N94" s="30"/>
     </row>
     <row r="95" spans="1:27" ht="32" x14ac:dyDescent="0.2">
       <c r="A95" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="B95" s="4" t="s">
-        <v>415</v>
-      </c>
-      <c r="C95" s="5" t="s">
-        <v>416</v>
+        <v>393</v>
+      </c>
+      <c r="B95" s="4"/>
+      <c r="C95" s="14" t="s">
+        <v>28</v>
       </c>
       <c r="D95" s="4" t="s">
+        <v>409</v>
+      </c>
+      <c r="E95" s="4" t="s">
+        <v>410</v>
+      </c>
+      <c r="F95" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="G95" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="H95" s="4">
+        <v>2000</v>
+      </c>
+      <c r="I95" s="4">
+        <v>2015</v>
+      </c>
+      <c r="J95" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="K95" s="8" t="s">
+        <v>27</v>
+      </c>
+      <c r="L95" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="M95" s="7" t="s">
+        <v>411</v>
+      </c>
+      <c r="N95" s="28"/>
+    </row>
+    <row r="96" spans="1:27" ht="32" x14ac:dyDescent="0.2">
+      <c r="A96" s="4" t="s">
+        <v>393</v>
+      </c>
+      <c r="B96" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C96" s="5" t="s">
+        <v>413</v>
+      </c>
+      <c r="D96" s="4" t="s">
+        <v>296</v>
+      </c>
+      <c r="E96" s="4" t="s">
+        <v>486</v>
+      </c>
+      <c r="F96" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="G96" s="4" t="s">
         <v>299</v>
       </c>
-      <c r="E95" s="4" t="s">
-        <v>489</v>
-      </c>
-      <c r="F95" s="5" t="s">
-        <v>301</v>
-      </c>
-      <c r="G95" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="H95" s="4">
+      <c r="H96" s="4">
         <v>2011</v>
       </c>
-      <c r="I95" s="4">
+      <c r="I96" s="4">
         <v>2011</v>
       </c>
-      <c r="J95" s="4"/>
-      <c r="K95" s="8" t="s">
-        <v>417</v>
-      </c>
-      <c r="L95" s="7"/>
-      <c r="M95" s="7"/>
-      <c r="N95" s="29"/>
-    </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A96" s="4" t="s">
-        <v>396</v>
-      </c>
-      <c r="B96" s="4" t="s">
-        <v>415</v>
-      </c>
-      <c r="C96" s="5" t="s">
-        <v>418</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="E96" s="4" t="s">
-        <v>419</v>
-      </c>
-      <c r="F96" s="5" t="s">
-        <v>420</v>
-      </c>
-      <c r="G96" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="H96" s="4">
-        <v>2008</v>
-      </c>
-      <c r="I96" s="4">
-        <v>2012</v>
-      </c>
       <c r="J96" s="4"/>
-      <c r="K96" s="5" t="s">
-        <v>421</v>
+      <c r="K96" s="8" t="s">
+        <v>414</v>
       </c>
       <c r="L96" s="7"/>
       <c r="M96" s="7"/>
-      <c r="N96" s="29"/>
-    </row>
-    <row r="97" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="N96" s="28"/>
+    </row>
+    <row r="97" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A97" s="4" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B97" s="4" t="s">
+        <v>412</v>
+      </c>
+      <c r="C97" s="5" t="s">
         <v>415</v>
       </c>
-      <c r="C97" s="5" t="s">
-        <v>422</v>
-      </c>
       <c r="D97" s="4" t="s">
-        <v>486</v>
+        <v>416</v>
       </c>
       <c r="E97" s="4" t="s">
-        <v>423</v>
+        <v>416</v>
       </c>
       <c r="F97" s="5" t="s">
-        <v>422</v>
+        <v>417</v>
       </c>
       <c r="G97" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="H97" s="4"/>
-      <c r="I97" s="4"/>
+      <c r="H97" s="4">
+        <v>2008</v>
+      </c>
+      <c r="I97" s="4">
+        <v>2012</v>
+      </c>
       <c r="J97" s="4"/>
-      <c r="K97" s="5"/>
+      <c r="K97" s="5" t="s">
+        <v>418</v>
+      </c>
       <c r="L97" s="7"/>
       <c r="M97" s="7"/>
-      <c r="N97" s="29"/>
+      <c r="N97" s="28"/>
     </row>
     <row r="98" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A98" s="4" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B98" s="4" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C98" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="D98" s="4" t="s">
-        <v>425</v>
+        <v>483</v>
       </c>
       <c r="E98" s="4" t="s">
-        <v>490</v>
+        <v>420</v>
       </c>
       <c r="F98" s="5" t="s">
-        <v>424</v>
+        <v>419</v>
       </c>
       <c r="G98" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H98" s="4"/>
-      <c r="I98" s="4">
-        <v>1983</v>
-      </c>
+      <c r="I98" s="4"/>
       <c r="J98" s="4"/>
-      <c r="K98" s="5" t="s">
-        <v>401</v>
-      </c>
+      <c r="K98" s="5"/>
       <c r="L98" s="7"/>
       <c r="M98" s="7"/>
-      <c r="N98" s="29"/>
-    </row>
-    <row r="99" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="N98" s="28"/>
+    </row>
+    <row r="99" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A99" s="4" t="s">
-        <v>396</v>
+        <v>393</v>
       </c>
       <c r="B99" s="4" t="s">
-        <v>415</v>
+        <v>412</v>
       </c>
       <c r="C99" s="5" t="s">
-        <v>426</v>
+        <v>421</v>
       </c>
       <c r="D99" s="4" t="s">
+        <v>422</v>
+      </c>
+      <c r="E99" s="4" t="s">
         <v>487</v>
       </c>
-      <c r="E99" s="4" t="s">
-        <v>488</v>
-      </c>
       <c r="F99" s="5" t="s">
-        <v>427</v>
+        <v>421</v>
       </c>
       <c r="G99" s="4" t="s">
         <v>17</v>
       </c>
       <c r="H99" s="4"/>
-      <c r="I99" s="4" t="s">
-        <v>428</v>
+      <c r="I99" s="4">
+        <v>1983</v>
       </c>
       <c r="J99" s="4"/>
-      <c r="K99" s="5"/>
+      <c r="K99" s="5" t="s">
+        <v>398</v>
+      </c>
       <c r="L99" s="7"/>
       <c r="M99" s="7"/>
-      <c r="N99" s="29"/>
-      <c r="O99" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="100" spans="1:15" ht="32" x14ac:dyDescent="0.2">
+      <c r="N99" s="28"/>
+    </row>
+    <row r="100" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A100" s="4" t="s">
-        <v>429</v>
-      </c>
-      <c r="B100" s="4"/>
+        <v>393</v>
+      </c>
+      <c r="B100" s="4" t="s">
+        <v>412</v>
+      </c>
       <c r="C100" s="5" t="s">
-        <v>430</v>
+        <v>423</v>
       </c>
       <c r="D100" s="4" t="s">
-        <v>431</v>
+        <v>484</v>
       </c>
       <c r="E100" s="4" t="s">
-        <v>491</v>
+        <v>485</v>
       </c>
       <c r="F100" s="5" t="s">
-        <v>432</v>
+        <v>424</v>
       </c>
       <c r="G100" s="4" t="s">
-        <v>302</v>
-      </c>
-      <c r="H100" s="4">
-        <v>2011</v>
-      </c>
-      <c r="I100" s="4">
-        <v>2015</v>
+        <v>17</v>
+      </c>
+      <c r="H100" s="4"/>
+      <c r="I100" s="4" t="s">
+        <v>425</v>
       </c>
       <c r="J100" s="4"/>
-      <c r="K100" s="5" t="s">
-        <v>330</v>
-      </c>
+      <c r="K100" s="5"/>
       <c r="L100" s="7"/>
-      <c r="M100" s="7" t="s">
-        <v>492</v>
-      </c>
-      <c r="N100" s="29"/>
+      <c r="M100" s="7"/>
+      <c r="N100" s="28"/>
       <c r="O100" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="101" spans="1:15" x14ac:dyDescent="0.2">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="101" spans="1:15" ht="32" x14ac:dyDescent="0.2">
       <c r="A101" s="4" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B101" s="4"/>
       <c r="C101" s="5" t="s">
-        <v>433</v>
+        <v>427</v>
       </c>
       <c r="D101" s="4" t="s">
-        <v>434</v>
+        <v>428</v>
       </c>
       <c r="E101" s="4" t="s">
-        <v>435</v>
+        <v>488</v>
       </c>
       <c r="F101" s="5" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="G101" s="4" t="s">
-        <v>17</v>
+        <v>299</v>
       </c>
       <c r="H101" s="4">
         <v>2011</v>
@@ -5480,28 +5731,33 @@
       </c>
       <c r="J101" s="4"/>
       <c r="K101" s="5" t="s">
-        <v>437</v>
+        <v>327</v>
       </c>
       <c r="L101" s="7"/>
-      <c r="M101" s="7"/>
-      <c r="N101" s="29"/>
-    </row>
-    <row r="102" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="M101" s="7" t="s">
+        <v>489</v>
+      </c>
+      <c r="N101" s="28"/>
+      <c r="O101" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="102" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A102" s="4" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B102" s="4"/>
       <c r="C102" s="5" t="s">
-        <v>438</v>
+        <v>430</v>
       </c>
       <c r="D102" s="4" t="s">
-        <v>439</v>
+        <v>431</v>
       </c>
       <c r="E102" s="4" t="s">
-        <v>498</v>
+        <v>432</v>
       </c>
       <c r="F102" s="5" t="s">
-        <v>440</v>
+        <v>433</v>
       </c>
       <c r="G102" s="4" t="s">
         <v>17</v>
@@ -5514,54 +5770,88 @@
       </c>
       <c r="J102" s="4"/>
       <c r="K102" s="5" t="s">
-        <v>485</v>
+        <v>434</v>
       </c>
       <c r="L102" s="7"/>
-      <c r="M102" s="8" t="s">
-        <v>481</v>
-      </c>
-      <c r="N102" s="31"/>
-      <c r="O102" t="s">
-        <v>480</v>
-      </c>
+      <c r="M102" s="7"/>
+      <c r="N102" s="28"/>
     </row>
     <row r="103" spans="1:15" ht="48" x14ac:dyDescent="0.2">
       <c r="A103" s="4" t="s">
-        <v>429</v>
+        <v>426</v>
       </c>
       <c r="B103" s="4"/>
       <c r="C103" s="5" t="s">
-        <v>441</v>
+        <v>435</v>
       </c>
       <c r="D103" s="4" t="s">
-        <v>442</v>
+        <v>436</v>
       </c>
       <c r="E103" s="4" t="s">
-        <v>443</v>
+        <v>495</v>
       </c>
       <c r="F103" s="5" t="s">
-        <v>444</v>
-      </c>
-      <c r="G103" s="4"/>
+        <v>437</v>
+      </c>
+      <c r="G103" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="H103" s="4">
-        <v>2010</v>
+        <v>2011</v>
       </c>
       <c r="I103" s="4">
         <v>2015</v>
       </c>
       <c r="J103" s="4"/>
       <c r="K103" s="5" t="s">
-        <v>485</v>
-      </c>
-      <c r="L103" s="7" t="s">
+        <v>482</v>
+      </c>
+      <c r="L103" s="7"/>
+      <c r="M103" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="N103" s="30"/>
+      <c r="O103" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="104" spans="1:15" ht="48" x14ac:dyDescent="0.2">
+      <c r="A104" s="4" t="s">
+        <v>426</v>
+      </c>
+      <c r="B104" s="4"/>
+      <c r="C104" s="5" t="s">
+        <v>438</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>439</v>
+      </c>
+      <c r="E104" s="4" t="s">
+        <v>440</v>
+      </c>
+      <c r="F104" s="5" t="s">
+        <v>441</v>
+      </c>
+      <c r="G104" s="4"/>
+      <c r="H104" s="4">
+        <v>2010</v>
+      </c>
+      <c r="I104" s="4">
+        <v>2015</v>
+      </c>
+      <c r="J104" s="4"/>
+      <c r="K104" s="5" t="s">
+        <v>482</v>
+      </c>
+      <c r="L104" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="M103" s="8" t="s">
-        <v>481</v>
-      </c>
-      <c r="N103" s="31"/>
-      <c r="O103" t="s">
-        <v>480</v>
+      <c r="M104" s="8" t="s">
+        <v>478</v>
+      </c>
+      <c r="N104" s="30"/>
+      <c r="O104" t="s">
+        <v>477</v>
       </c>
     </row>
   </sheetData>
@@ -5574,10 +5864,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5587,7 +5877,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="C1" t="s">
         <v>11</v>
@@ -5595,57 +5885,90 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>415</v>
-      </c>
-      <c r="B2" s="34" t="s">
-        <v>495</v>
+        <v>412</v>
+      </c>
+      <c r="B2" s="33" t="s">
+        <v>492</v>
       </c>
       <c r="C2" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>491</v>
+      </c>
+      <c r="B3" s="33" t="s">
+        <v>492</v>
+      </c>
+      <c r="C3" t="s">
         <v>494</v>
-      </c>
-      <c r="B3" s="34" t="s">
-        <v>495</v>
-      </c>
-      <c r="C3" t="s">
-        <v>497</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B4" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="C4" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B5" t="s">
+        <v>497</v>
+      </c>
+      <c r="C5" t="s">
         <v>500</v>
-      </c>
-      <c r="C5" t="s">
-        <v>503</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>505</v>
+        <v>502</v>
       </c>
       <c r="B6" t="s">
-        <v>506</v>
+        <v>503</v>
       </c>
       <c r="C6" t="s">
-        <v>507</v>
+        <v>504</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>501</v>
+      </c>
+      <c r="B7" t="s">
+        <v>550</v>
+      </c>
+      <c r="C7" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>551</v>
+      </c>
+      <c r="B8" t="s">
+        <v>552</v>
+      </c>
+      <c r="C8" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>551</v>
+      </c>
+      <c r="B9" t="s">
+        <v>555</v>
+      </c>
+      <c r="C9" t="s">
+        <v>556</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated cp and hab extent with fishpond, reef extent, soft-bottom, and wetlands extent
</commit_message>
<xml_diff>
--- a/prep_whi/data_layers_WH.xlsx
+++ b/prep_whi/data_layers_WH.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3360" yWindow="1260" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data_layers_WH.csv" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="889" uniqueCount="557">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="559">
   <si>
     <t>Goal</t>
   </si>
@@ -1699,6 +1699,12 @@
   </si>
   <si>
     <t xml:space="preserve">updated cp_extent layer updated, need to updated mhi reef exent layer </t>
+  </si>
+  <si>
+    <t xml:space="preserve">updated hab_extent data layer </t>
+  </si>
+  <si>
+    <t>updated cp_extent data layer for fishponds using fishpond layer from Joey (old TNC layer)</t>
   </si>
 </sst>
 </file>
@@ -5864,10 +5870,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5971,6 +5977,28 @@
         <v>556</v>
       </c>
     </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>551</v>
+      </c>
+      <c r="B10" t="s">
+        <v>555</v>
+      </c>
+      <c r="C10" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>551</v>
+      </c>
+      <c r="B11" t="s">
+        <v>555</v>
+      </c>
+      <c r="C11" t="s">
+        <v>558</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updated mar data layers for West Hawaii
</commit_message>
<xml_diff>
--- a/prep_whi/data_layers_WH.xlsx
+++ b/prep_whi/data_layers_WH.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3360" yWindow="1260" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="3400" yWindow="1960" windowWidth="28800" windowHeight="16740" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="data_layers_WH.csv" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="895" uniqueCount="559">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="910" uniqueCount="565">
   <si>
     <t>Goal</t>
   </si>
@@ -1705,6 +1705,24 @@
   </si>
   <si>
     <t>updated cp_extent data layer for fishponds using fishpond layer from Joey (old TNC layer)</t>
+  </si>
+  <si>
+    <t>12/28/2017</t>
+  </si>
+  <si>
+    <t>emailed Jonathan Page UHERO for data on subcounty livelihoods and economies</t>
+  </si>
+  <si>
+    <t>updated fishpond layers with current km2 of fishponds in each region, #, and status (current area/historical area) using old fishpond layer</t>
+  </si>
+  <si>
+    <t>updated MAR goal - NELHA is split between N and S regions - propose we use the same score for opperators and aquaculture for both N and S as a subet of the goal score of aquaculture and fishponds</t>
+  </si>
+  <si>
+    <t>need to adjust shellfish operators and include mullusk operators as a seprate entry as there is different risk for shrimp vs abolone and he'e</t>
+  </si>
+  <si>
+    <t>most of the industry is in tourism and recreation - use proxy of hotels and occupancy for weighting between regions and split the living resources between both regions</t>
   </si>
 </sst>
 </file>
@@ -5870,10 +5888,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -5999,6 +6017,61 @@
         <v>558</v>
       </c>
     </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>149</v>
+      </c>
+      <c r="B12" t="s">
+        <v>559</v>
+      </c>
+      <c r="C12" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" t="s">
+        <v>133</v>
+      </c>
+      <c r="B13" t="s">
+        <v>559</v>
+      </c>
+      <c r="C13" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A14" t="s">
+        <v>133</v>
+      </c>
+      <c r="B14" t="s">
+        <v>559</v>
+      </c>
+      <c r="C14" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A15" t="s">
+        <v>133</v>
+      </c>
+      <c r="B15" t="s">
+        <v>559</v>
+      </c>
+      <c r="C15" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A16" t="s">
+        <v>149</v>
+      </c>
+      <c r="B16" t="s">
+        <v>559</v>
+      </c>
+      <c r="C16" t="s">
+        <v>564</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>